<commit_message>
Half way through running tests for cran with no title
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="MAP Scores" sheetId="1" r:id="rId1"/>
-    <sheet name="Datasets" sheetId="4" r:id="rId2"/>
+    <sheet name="MAP Scores - Cran" sheetId="5" r:id="rId1"/>
+    <sheet name="MAP Scores - Cran Title" sheetId="1" r:id="rId2"/>
+    <sheet name="Datasets" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Unmodified Cosine</t>
   </si>
@@ -179,6 +180,78 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Cran - Title</t>
+  </si>
+  <si>
+    <t>Cran- No Title</t>
+  </si>
+  <si>
+    <t>sub idf bottom=5 prob=.25</t>
+  </si>
+  <si>
+    <t>noun i=0.8</t>
+  </si>
+  <si>
+    <t>adj i=0.8</t>
+  </si>
+  <si>
+    <t>verb i=0.4</t>
+  </si>
+  <si>
+    <t>adv i=0.8</t>
+  </si>
+  <si>
+    <t>Time MAP</t>
+  </si>
+  <si>
+    <t>Trained on Cran with Title</t>
+  </si>
+  <si>
+    <t>Trained on Cran without Title</t>
+  </si>
+  <si>
+    <t>sub all prob=.1</t>
+  </si>
+  <si>
+    <t>early adj i=1.4</t>
+  </si>
+  <si>
+    <t>early adv i=1.4</t>
+  </si>
+  <si>
+    <t>early all i=2.2</t>
+  </si>
+  <si>
+    <t>early not verb i=2.6</t>
+  </si>
+  <si>
+    <t>early noun i=1.6</t>
+  </si>
+  <si>
+    <t>early adj noun  i=2.6</t>
+  </si>
+  <si>
+    <t>early adv verb i=1.2</t>
+  </si>
+  <si>
+    <t>early not adj i=1.6</t>
+  </si>
+  <si>
+    <t>sub noun prob=.02</t>
+  </si>
+  <si>
+    <t>sub verb prob=.06</t>
+  </si>
+  <si>
+    <t>early not adv i=2.2</t>
+  </si>
+  <si>
+    <t>early not adv verb  i=2.6</t>
   </si>
 </sst>
 </file>
@@ -190,7 +263,7 @@
     <numFmt numFmtId="165" formatCode="0.000%"/>
     <numFmt numFmtId="173" formatCode="0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,8 +312,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,8 +381,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -327,6 +419,19 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -349,6 +454,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -467,7 +587,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -581,8 +701,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -598,7 +732,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="173" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -610,89 +750,77 @@
     <xf numFmtId="173" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="173" fontId="4" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="7" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="7" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="4" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="173" fontId="4" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -701,42 +829,42 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="173" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="173" fontId="4" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="4" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="4" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="9" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="173" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -769,8 +897,35 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="127">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -827,6 +982,13 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -882,6 +1044,13 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1212,923 +1381,2527 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="23">
+      <c r="A1" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" ht="61" thickBot="1">
+      <c r="A2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19" thickTop="1">
+      <c r="A3" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="56">
+        <v>0.238436125225614</v>
+      </c>
+      <c r="C3" s="57">
+        <f>(B3-$B$4)/$B$4</f>
+        <v>-2.2047539075231905E-2</v>
+      </c>
+      <c r="D3" s="58"/>
+      <c r="E3" s="57" t="e">
+        <f>(D3-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3" s="58"/>
+      <c r="G3" s="57" t="e">
+        <f>(F3-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H3" s="58"/>
+      <c r="I3" s="77" t="e">
+        <f>(H3-$H$4)/$H$4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18">
+      <c r="A4" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="60">
+        <v>0.24381157034989701</v>
+      </c>
+      <c r="C4" s="61">
+        <f>(B4-$B$4)/$B$4</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="62"/>
+      <c r="E4" s="61" t="e">
+        <f>(D4-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4" s="62"/>
+      <c r="G4" s="61" t="e">
+        <f>(F4-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4" s="62"/>
+      <c r="I4" s="77" t="e">
+        <f>(H4-$H$4)/$H$4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18">
+      <c r="A5" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="40">
+        <v>0.243523296438478</v>
+      </c>
+      <c r="C5" s="15">
+        <f>(B5-$B$4)/$B$4</f>
+        <v>-1.1823635400292772E-3</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="15" t="e">
+        <f>(D5-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="41"/>
+      <c r="G5" s="15" t="e">
+        <f>(F5-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="10" t="e">
+        <f t="shared" ref="I5:I40" si="0">(H5-$H$4)/$H$4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18">
+      <c r="A6" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="40">
+        <v>0.24364250981777499</v>
+      </c>
+      <c r="C6" s="15">
+        <f>(B6-$B$4)/$B$4</f>
+        <v>-6.9340651831818691E-4</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="15" t="e">
+        <f>(D6-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="15" t="e">
+        <f>(F6-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="41"/>
+      <c r="I6" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18">
+      <c r="A7" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="40">
+        <v>0.243809826790511</v>
+      </c>
+      <c r="C7" s="15">
+        <f>(B7-$B$4)/$B$4</f>
+        <v>-7.1512577664219435E-6</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="15" t="e">
+        <f>(D7-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="15" t="e">
+        <f>(F7-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="41"/>
+      <c r="I7" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18">
+      <c r="A8" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="15">
+        <f>(B8-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D8" s="41"/>
+      <c r="E8" s="15" t="e">
+        <f>(D8-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="15" t="e">
+        <f>(F8-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="41"/>
+      <c r="I8" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="40"/>
+      <c r="C9" s="15">
+        <f>(B9-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D9" s="41"/>
+      <c r="E9" s="15" t="e">
+        <f>(D9-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="15" t="e">
+        <f>(F9-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="41"/>
+      <c r="I9" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18">
+      <c r="A10" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="40"/>
+      <c r="C10" s="15">
+        <f>(B10-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="15" t="e">
+        <f>(D10-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" s="41"/>
+      <c r="G10" s="15" t="e">
+        <f>(F10-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="41"/>
+      <c r="I10" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18">
+      <c r="A11" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="15">
+        <f>(B11-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D11" s="41"/>
+      <c r="E11" s="15" t="e">
+        <f>(D11-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="41"/>
+      <c r="G11" s="15" t="e">
+        <f>(F11-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="41"/>
+      <c r="I11" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18">
+      <c r="A12" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="44">
+        <v>0.20670779224481001</v>
+      </c>
+      <c r="C12" s="45">
+        <f>(B12-$B$4)/$B$4</f>
+        <v>-0.15218218746484799</v>
+      </c>
+      <c r="D12" s="46"/>
+      <c r="E12" s="45" t="e">
+        <f>(D12-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="46"/>
+      <c r="G12" s="45" t="e">
+        <f>(F12-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="46"/>
+      <c r="I12" s="81" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18">
+      <c r="A13" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="48">
+        <v>0.24353295067911801</v>
+      </c>
+      <c r="C13" s="49">
+        <f>(B13-$B$4)/$B$4</f>
+        <v>-1.142766401033163E-3</v>
+      </c>
+      <c r="D13" s="50"/>
+      <c r="E13" s="49" t="e">
+        <f>(D13-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="50"/>
+      <c r="G13" s="49" t="e">
+        <f>(F13-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="50"/>
+      <c r="I13" s="81" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18">
+      <c r="A14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="19">
+        <v>0.25156069135867398</v>
+      </c>
+      <c r="C14" s="17">
+        <f>(B14-$B$4)/$B$4</f>
+        <v>3.1783237348646402E-2</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="17" t="e">
+        <f>(D14-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="17" t="e">
+        <f>(F14-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18">
+      <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0.25046477420976698</v>
+      </c>
+      <c r="C15" s="17">
+        <f>(B15-$B$4)/$B$4</f>
+        <v>2.7288302398126067E-2</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="17" t="e">
+        <f>(D15-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="17" t="e">
+        <f>(F15-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="13"/>
+      <c r="I15" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18">
+      <c r="A16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="20">
+        <v>0.247419697024271</v>
+      </c>
+      <c r="C16" s="17">
+        <f>(B16-$B$4)/$B$4</f>
+        <v>1.4798832841263125E-2</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="17" t="e">
+        <f>(D16-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="17" t="e">
+        <f>(F16-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="20">
+        <v>0.245402577321679</v>
+      </c>
+      <c r="C17" s="17">
+        <f>(B17-$B$4)/$B$4</f>
+        <v>6.5255597570645241E-3</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="17" t="e">
+        <f>(D17-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="G17" s="17" t="e">
+        <f>(F17-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18">
+      <c r="A18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="20">
+        <v>0.24552897807379301</v>
+      </c>
+      <c r="C18" s="17">
+        <f>(B18-$B$4)/$B$4</f>
+        <v>7.0439959901465289E-3</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="17" t="e">
+        <f>(D18-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="17" t="e">
+        <f>(F18-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H18" s="13"/>
+      <c r="I18" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18">
+      <c r="A19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="20">
+        <v>0.25372541704894802</v>
+      </c>
+      <c r="C19" s="17">
+        <f>(B19-$B$4)/$B$4</f>
+        <v>4.0661920534876717E-2</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="17" t="e">
+        <f>(D19-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="G19" s="17" t="e">
+        <f>(F19-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18">
+      <c r="A20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="20">
+        <v>0.24672743114774001</v>
+      </c>
+      <c r="C20" s="17">
+        <f>(B20-$B$4)/$B$4</f>
+        <v>1.1959484915578118E-2</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="17" t="e">
+        <f>(D20-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="17" t="e">
+        <f>(F20-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.24820233481440501</v>
+      </c>
+      <c r="C21" s="17">
+        <f>(B21-$B$4)/$B$4</f>
+        <v>1.8008843707485934E-2</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="17" t="e">
+        <f>(D21-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="17" t="e">
+        <f>(F21-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18">
+      <c r="A22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.24699614031921799</v>
+      </c>
+      <c r="C22" s="17">
+        <f>(B22-$B$4)/$B$4</f>
+        <v>1.3061603125523399E-2</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="17" t="e">
+        <f>(D22-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="17" t="e">
+        <f>(F22-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18">
+      <c r="A23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0.25281148825765098</v>
+      </c>
+      <c r="C23" s="17">
+        <f>(B23-$B$4)/$B$4</f>
+        <v>3.6913415941819683E-2</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="17" t="e">
+        <f>(D23-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="17" t="e">
+        <f>(F23-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18">
+      <c r="A24" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="19">
+        <v>0.251392039102381</v>
+      </c>
+      <c r="C24" s="17">
+        <f>(B24-$B$4)/$B$4</f>
+        <v>3.1091505385102004E-2</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="17" t="e">
+        <f>(D24-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="17" t="e">
+        <f>(F24-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H24" s="12"/>
+      <c r="I24" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18">
+      <c r="A25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="19">
+        <v>0.25303892731352501</v>
+      </c>
+      <c r="C25" s="17">
+        <f>(B25-$B$4)/$B$4</f>
+        <v>3.7846263614092261E-2</v>
+      </c>
+      <c r="D25" s="12"/>
+      <c r="E25" s="17" t="e">
+        <f>(D25-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="17" t="e">
+        <f>(F25-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18">
+      <c r="A26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="21">
+        <v>0.246826309053788</v>
+      </c>
+      <c r="C26" s="18">
+        <f>(B26-$B$4)/$B$4</f>
+        <v>1.236503542290672E-2</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="18" t="e">
+        <f>(D26-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="18" t="e">
+        <f>(F26-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H26" s="14"/>
+      <c r="I26" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18">
+      <c r="A27" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27">
+        <f>(B27-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D27" s="63"/>
+      <c r="E27" s="27" t="e">
+        <f>(D27-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F27" s="63"/>
+      <c r="G27" s="27" t="e">
+        <f>(F27-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H27" s="63"/>
+      <c r="I27" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18">
+      <c r="A28" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27">
+        <f>(B28-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D28" s="63"/>
+      <c r="E28" s="27" t="e">
+        <f>(D28-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F28" s="63"/>
+      <c r="G28" s="27" t="e">
+        <f>(F28-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="63"/>
+      <c r="I28" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18">
+      <c r="A29" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27">
+        <f>(B29-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D29" s="63"/>
+      <c r="E29" s="27" t="e">
+        <f>(D29-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="63"/>
+      <c r="G29" s="27" t="e">
+        <f>(F29-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="63"/>
+      <c r="I29" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18">
+      <c r="A30" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="27">
+        <f>(B30-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D30" s="75"/>
+      <c r="E30" s="27" t="e">
+        <f>(D30-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" s="75"/>
+      <c r="G30" s="27" t="e">
+        <f>(F30-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H30" s="75"/>
+      <c r="I30" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18">
+      <c r="A31" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="27">
+        <f>(B31-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D31" s="63"/>
+      <c r="E31" s="27" t="e">
+        <f>(D31-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F31" s="63"/>
+      <c r="G31" s="27" t="e">
+        <f>(F31-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="63"/>
+      <c r="I31" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18">
+      <c r="A32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="27">
+        <f>(B32-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D32" s="63"/>
+      <c r="E32" s="27" t="e">
+        <f>(D32-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F32" s="63"/>
+      <c r="G32" s="27" t="e">
+        <f>(F32-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H32" s="63"/>
+      <c r="I32" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18">
+      <c r="A33" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="27">
+        <f>(B33-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D33" s="63"/>
+      <c r="E33" s="27" t="e">
+        <f>(D33-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F33" s="63"/>
+      <c r="G33" s="27" t="e">
+        <f>(F33-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H33" s="63"/>
+      <c r="I33" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18">
+      <c r="A34" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="31">
+        <f>(B34-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D34" s="64"/>
+      <c r="E34" s="31" t="e">
+        <f>(D34-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F34" s="64"/>
+      <c r="G34" s="31" t="e">
+        <f>(F34-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H34" s="64"/>
+      <c r="I34" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="52">
+        <v>0.242987098680572</v>
+      </c>
+      <c r="C35" s="16">
+        <f>(B35-$B$4)/$B$4</f>
+        <v>-3.3815936960735534E-3</v>
+      </c>
+      <c r="D35" s="65"/>
+      <c r="E35" s="16" t="e">
+        <f>(D35-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F35" s="65"/>
+      <c r="G35" s="16" t="e">
+        <f>(F35-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H35" s="65"/>
+      <c r="I35" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18">
+      <c r="A36" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="52"/>
+      <c r="C36" s="16">
+        <f>(B36-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D36" s="65"/>
+      <c r="E36" s="16" t="e">
+        <f>(D36-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F36" s="65"/>
+      <c r="G36" s="16" t="e">
+        <f>(F36-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H36" s="65"/>
+      <c r="I36" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="18">
+      <c r="A37" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="54"/>
+      <c r="C37" s="22">
+        <f>(B37-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D37" s="66"/>
+      <c r="E37" s="22" t="e">
+        <f>(D37-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F37" s="66"/>
+      <c r="G37" s="22" t="e">
+        <f>(F37-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H37" s="66"/>
+      <c r="I37" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="18">
+      <c r="A38" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34">
+        <f>(B38-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D38" s="67"/>
+      <c r="E38" s="34" t="e">
+        <f>(D38-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F38" s="67"/>
+      <c r="G38" s="34" t="e">
+        <f>(F38-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H38" s="67"/>
+      <c r="I38" s="80" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18">
+      <c r="A39" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="34">
+        <f>(B39-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D39" s="67"/>
+      <c r="E39" s="34" t="e">
+        <f>(D39-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F39" s="67"/>
+      <c r="G39" s="34" t="e">
+        <f>(F39-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H39" s="67"/>
+      <c r="I39" s="80" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18">
+      <c r="A40" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38">
+        <f>(B40-$B$4)/$B$4</f>
+        <v>-1</v>
+      </c>
+      <c r="D40" s="68"/>
+      <c r="E40" s="38" t="e">
+        <f>(D40-$D$4)/$D$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F40" s="68"/>
+      <c r="G40" s="38" t="e">
+        <f>(F40-$F$4)/$F$4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H40" s="68"/>
+      <c r="I40" s="80" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="7" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="41" thickBot="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:9" ht="32" customHeight="1">
+      <c r="A1" s="76" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="41" thickBot="1">
+      <c r="A2" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="19" thickTop="1">
-      <c r="A2" s="57" t="s">
+      <c r="H2" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19" thickTop="1">
+      <c r="A3" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B3" s="56">
         <v>0.28156330866837298</v>
       </c>
-      <c r="C2" s="59">
-        <f>(B2-$B$3)/$B$3</f>
+      <c r="C3" s="57">
+        <f>(B3-$B$4)/$B$4</f>
         <v>-1.2869678140698165E-3</v>
       </c>
-      <c r="D2" s="60">
+      <c r="D3" s="58">
         <v>0.377836663007103</v>
       </c>
-      <c r="E2" s="59">
-        <f t="shared" ref="E2:E3" si="0">(D2-$D$3)/$D$3</f>
+      <c r="E3" s="57">
+        <f>(D3-$D$4)/$D$4</f>
         <v>-2.9845911176526658E-3</v>
       </c>
-      <c r="F2" s="60">
+      <c r="F3" s="58">
         <v>0.52990836804548702</v>
       </c>
-      <c r="G2" s="59">
-        <f t="shared" ref="G2:G34" si="1">(F2-$F$3)/$F$3</f>
+      <c r="G3" s="57">
+        <f>(F3-$F$4)/$F$4</f>
         <v>-8.6415438489028037E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="18">
-      <c r="A3" s="61" t="s">
+      <c r="H3" s="58">
+        <v>1.2091846347657E-2</v>
+      </c>
+      <c r="I3" s="77">
+        <f>(H3-$H$4)/$H$4</f>
+        <v>-6.0369296183416854E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18">
+      <c r="A4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B4" s="60">
         <v>0.28192613853461201</v>
       </c>
-      <c r="C3" s="63">
-        <f>(B3-$B$3)/$B$3</f>
+      <c r="C4" s="61">
+        <f>(B4-$B$4)/$B$4</f>
         <v>0</v>
       </c>
-      <c r="D3" s="64">
+      <c r="D4" s="62">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E3" s="63">
-        <f t="shared" si="0"/>
+      <c r="E4" s="61">
+        <f>(D4-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F3" s="64">
+      <c r="F4" s="62">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G3" s="63">
-        <f t="shared" si="1"/>
+      <c r="G4" s="61">
+        <f>(F4-$F$4)/$F$4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="18">
-      <c r="A4" s="41" t="s">
+      <c r="H4" s="62">
+        <v>1.2868722039991299E-2</v>
+      </c>
+      <c r="I4" s="77">
+        <f t="shared" ref="I4:I40" si="0">(H4-$H$4)/$H$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18">
+      <c r="A5" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="42">
+      <c r="B5" s="40">
         <v>0.28184556317065801</v>
       </c>
-      <c r="C4" s="13">
-        <f>(B4-$B$3)/$B$3</f>
+      <c r="C5" s="15">
+        <f>(B5-$B$4)/$B$4</f>
         <v>-2.8580309854495095E-4</v>
       </c>
-      <c r="D4" s="43">
+      <c r="D5" s="41">
         <v>0.37843201243242902</v>
       </c>
-      <c r="E4" s="13">
-        <f>(D4-$D$3)/$D$3</f>
+      <c r="E5" s="15">
+        <f>(D5-$D$4)/$D$4</f>
         <v>-1.4136145321746885E-3</v>
       </c>
-      <c r="F4" s="43">
+      <c r="F5" s="41">
         <v>0.53529098731159497</v>
       </c>
-      <c r="G4" s="13">
-        <f>(F4-$F$3)/$F$3</f>
+      <c r="G5" s="15">
+        <f>(F5-$F$4)/$F$4</f>
         <v>1.4283200133713568E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="18">
-      <c r="A5" s="41" t="s">
+      <c r="H5" s="41">
+        <v>1.28676444518622E-2</v>
+      </c>
+      <c r="I5" s="10">
+        <f t="shared" si="0"/>
+        <v>-8.3736996241806999E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18">
+      <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="42">
+      <c r="B6" s="40">
         <v>0.28170329030443297</v>
       </c>
-      <c r="C5" s="13">
-        <f t="shared" ref="C5:C34" si="2">(B5-$B$3)/$B$3</f>
+      <c r="C6" s="15">
+        <f>(B6-$B$4)/$B$4</f>
         <v>-7.9044898545893843E-4</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D6" s="41">
         <v>0.37849153624195297</v>
       </c>
-      <c r="E5" s="13">
-        <f t="shared" ref="E5:G28" si="3">(D5-$D$3)/$D$3</f>
+      <c r="E6" s="15">
+        <f>(D6-$D$4)/$D$4</f>
         <v>-1.2565462508214735E-3</v>
       </c>
-      <c r="F5" s="43">
+      <c r="F6" s="41">
         <v>0.53439377687493905</v>
       </c>
-      <c r="G5" s="13">
-        <f t="shared" si="1"/>
+      <c r="G6" s="15">
+        <f>(F6-$F$4)/$F$4</f>
         <v>-2.501912292544805E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="18">
-      <c r="A6" s="41" t="s">
+      <c r="H6" s="41">
+        <v>1.2868244038268001E-2</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.7144459396439586E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="42">
+      <c r="B7" s="40">
         <v>0.28192613853461201</v>
       </c>
-      <c r="C6" s="13">
-        <f t="shared" si="2"/>
+      <c r="C7" s="15">
+        <f>(B7-$B$4)/$B$4</f>
         <v>0</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D7" s="41">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E6" s="13">
-        <f t="shared" si="3"/>
+      <c r="E7" s="15">
+        <f>(D7-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F7" s="41">
         <v>0.53482723871359905</v>
       </c>
-      <c r="G6" s="13">
-        <f t="shared" si="1"/>
+      <c r="G7" s="15">
+        <f>(F7-$F$4)/$F$4</f>
         <v>5.6073398930614742E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="41" t="s">
+      <c r="H7" s="41">
+        <v>1.2868122453585601E-2</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="0"/>
+        <v>-4.6592536837414126E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="42">
+      <c r="B8" s="40">
         <v>0.28206841140083799</v>
       </c>
-      <c r="C7" s="13">
-        <f t="shared" si="2"/>
+      <c r="C8" s="15">
+        <f>(B8-$B$4)/$B$4</f>
         <v>5.0464588691733479E-4</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D8" s="41">
         <v>0.37890820290861998</v>
       </c>
-      <c r="E7" s="13">
-        <f t="shared" si="3"/>
+      <c r="E8" s="15">
+        <f>(D8-$D$4)/$D$4</f>
         <v>-1.5706828135072501E-4</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F8" s="41">
         <v>0.53479525505563497</v>
       </c>
-      <c r="G7" s="13">
-        <f t="shared" si="1"/>
+      <c r="G8" s="15">
+        <f>(F8-$F$4)/$F$4</f>
         <v>5.0089860701488568E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="18">
-      <c r="A8" s="41" t="s">
+      <c r="H8" s="41">
+        <v>1.2868722039991299E-2</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18">
+      <c r="A9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B9" s="40">
         <v>0.28192613853461201</v>
       </c>
-      <c r="C8" s="13">
-        <f t="shared" si="2"/>
+      <c r="C9" s="15">
+        <f>(B9-$B$4)/$B$4</f>
         <v>0</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D9" s="41">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E8" s="13">
-        <f t="shared" si="3"/>
+      <c r="E9" s="15">
+        <f>(D9-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F9" s="41">
         <v>0.53471004279187295</v>
       </c>
-      <c r="G8" s="13">
-        <f t="shared" si="1"/>
+      <c r="G9" s="15">
+        <f>(F9-$F$4)/$F$4</f>
         <v>3.4148255823681029E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="18">
-      <c r="A9" s="44" t="s">
+      <c r="H9" s="41">
+        <v>1.2868722039991299E-2</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18">
+      <c r="A10" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="40">
+        <v>0.28198870051963898</v>
+      </c>
+      <c r="C10" s="15">
+        <f>(B10-$B$4)/$B$4</f>
+        <v>2.2190913319406421E-4</v>
+      </c>
+      <c r="D10" s="41">
+        <v>0.37849153624195297</v>
+      </c>
+      <c r="E10" s="15">
+        <f>(D10-$D$4)/$D$4</f>
+        <v>-1.2565462508214735E-3</v>
+      </c>
+      <c r="F10" s="41">
+        <v>0.53452751096997897</v>
+      </c>
+      <c r="G10" s="15">
+        <f>(F10-$F$4)/$F$4</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="41">
+        <v>1.2868122453585601E-2</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="0"/>
+        <v>-4.6592536837414126E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18">
+      <c r="A11" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="42">
+      <c r="B11" s="40">
         <v>0.28221558750820902</v>
       </c>
-      <c r="C9" s="13">
-        <f t="shared" si="2"/>
+      <c r="C11" s="15">
+        <f>(B11-$B$4)/$B$4</f>
         <v>1.0266837090788965E-3</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D11" s="41">
         <v>0.37890820290861998</v>
       </c>
-      <c r="E9" s="13">
-        <f t="shared" si="3"/>
+      <c r="E11" s="15">
+        <f>(D11-$D$4)/$D$4</f>
         <v>-1.5706828135072501E-4</v>
       </c>
-      <c r="F9" s="43">
+      <c r="F11" s="41">
         <v>0.53462223249454</v>
       </c>
-      <c r="G9" s="13">
-        <f t="shared" si="1"/>
+      <c r="G11" s="15">
+        <f>(F11-$F$4)/$F$4</f>
         <v>1.7720607941982142E-4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="18">
-      <c r="A10" s="45" t="s">
+      <c r="H11" s="41">
+        <v>1.2868244038268001E-2</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="0"/>
+        <v>-3.7144459396439586E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18">
+      <c r="A12" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B12" s="44">
         <v>0.22772938455928099</v>
       </c>
-      <c r="C10" s="47">
-        <f t="shared" si="2"/>
+      <c r="C12" s="45">
+        <f>(B12-$B$4)/$B$4</f>
         <v>-0.19223742167729971</v>
       </c>
-      <c r="D10" s="48">
+      <c r="D12" s="46">
         <v>0.345222250131828</v>
       </c>
-      <c r="E10" s="47">
-        <f t="shared" si="3"/>
+      <c r="E12" s="45">
+        <f>(D12-$D$4)/$D$4</f>
         <v>-8.904577938219306E-2</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F12" s="46">
         <v>0.49854150924888802</v>
       </c>
-      <c r="G10" s="47">
-        <f t="shared" si="1"/>
+      <c r="G12" s="45">
+        <f>(F12-$F$4)/$F$4</f>
         <v>-6.7323011412058195E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="18">
-      <c r="A11" s="49" t="s">
+      <c r="H12" s="46">
+        <v>1.380620281143E-2</v>
+      </c>
+      <c r="I12" s="77">
+        <f t="shared" si="0"/>
+        <v>7.2849562569255261E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18">
+      <c r="A13" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="50">
+      <c r="B13" s="48">
         <v>0.28132255653984201</v>
       </c>
-      <c r="C11" s="51">
-        <f t="shared" si="2"/>
+      <c r="C13" s="49">
+        <f>(B13-$B$4)/$B$4</f>
         <v>-2.1409224341782931E-3</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D13" s="50">
         <v>0.38526070879256302</v>
       </c>
-      <c r="E11" s="51">
-        <f t="shared" si="3"/>
+      <c r="E13" s="49">
+        <f>(D13-$D$4)/$D$4</f>
         <v>1.6605588367424304E-2</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F13" s="50">
         <v>0.535015149771215</v>
       </c>
-      <c r="G11" s="51">
-        <f t="shared" si="1"/>
+      <c r="G13" s="49">
+        <f>(F13-$F$4)/$F$4</f>
         <v>9.1228008143330532E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="18">
-      <c r="A12" s="3" t="s">
+      <c r="H13" s="50">
+        <v>1.27313006966878E-2</v>
+      </c>
+      <c r="I13" s="77">
+        <f t="shared" si="0"/>
+        <v>-1.0678709422461952E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18">
+      <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B14" s="19">
         <v>0.29653734494720901</v>
       </c>
-      <c r="C12" s="15">
-        <f t="shared" si="2"/>
+      <c r="C14" s="17">
+        <f>(B14-$B$4)/$B$4</f>
         <v>5.182636306283174E-2</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D14" s="12">
         <v>0.38438913315652201</v>
       </c>
-      <c r="E12" s="15">
-        <f t="shared" si="3"/>
+      <c r="E14" s="17">
+        <f>(D14-$D$4)/$D$4</f>
         <v>1.4305720662095284E-2</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F14" s="12">
         <v>0.55367549907609603</v>
       </c>
-      <c r="G12" s="15">
-        <f t="shared" si="1"/>
+      <c r="G14" s="17">
+        <f>(F14-$F$4)/$F$4</f>
         <v>3.5822268663721755E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="18">
-      <c r="A13" s="3" t="s">
+      <c r="H14" s="12">
+        <v>1.2015975246253099E-2</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.6265072094041158E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18">
+      <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B15" s="20">
         <v>0.288927228692064</v>
       </c>
-      <c r="C13" s="15">
-        <f t="shared" si="2"/>
+      <c r="C15" s="17">
+        <f>(B15-$B$4)/$B$4</f>
         <v>2.4833065120680398E-2</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D15" s="13">
         <v>0.37868122199941301</v>
       </c>
-      <c r="E13" s="15">
-        <f t="shared" si="3"/>
+      <c r="E15" s="17">
+        <f>(D15-$D$4)/$D$4</f>
         <v>-7.5601350334265503E-4</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F15" s="13">
         <v>0.54996186535253899</v>
       </c>
-      <c r="G13" s="15">
-        <f t="shared" si="1"/>
+      <c r="G15" s="17">
+        <f>(F15-$F$4)/$F$4</f>
         <v>2.8874761477762131E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="18">
-      <c r="A14" s="3" t="s">
+      <c r="H15" s="13">
+        <v>1.21386906875686E-2</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.6729125872330442E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18">
+      <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B16" s="20">
         <v>0.29046785478988502</v>
       </c>
-      <c r="C14" s="15">
-        <f t="shared" si="2"/>
+      <c r="C16" s="17">
+        <f>(B16-$B$4)/$B$4</f>
         <v>3.0297709533677514E-2</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D16" s="13">
         <v>0.37875368811124799</v>
       </c>
-      <c r="E14" s="15">
-        <f t="shared" si="3"/>
+      <c r="E16" s="17">
+        <f>(D16-$D$4)/$D$4</f>
         <v>-5.6479375895298147E-4</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F16" s="13">
         <v>0.534640541558564</v>
       </c>
-      <c r="G14" s="15">
-        <f t="shared" si="1"/>
+      <c r="G16" s="17">
+        <f>(F16-$F$4)/$F$4</f>
         <v>2.1145887959988691E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="18">
-      <c r="A15" s="3" t="s">
+      <c r="H16" s="13">
+        <v>1.35859384549026E-2</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="shared" si="0"/>
+        <v>5.5733305349393192E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B17" s="20">
         <v>0.28415653055485501</v>
       </c>
-      <c r="C15" s="15">
-        <f t="shared" si="2"/>
+      <c r="C17" s="17">
+        <f>(B17-$B$4)/$B$4</f>
         <v>7.9112636800407025E-3</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D17" s="13">
         <v>0.37669056162282799</v>
       </c>
-      <c r="E15" s="15">
-        <f t="shared" si="3"/>
+      <c r="E17" s="17">
+        <f>(D17-$D$4)/$D$4</f>
         <v>-6.008862852346906E-3</v>
       </c>
-      <c r="F15" s="11">
+      <c r="F17" s="13">
         <v>0.53532905335487102</v>
       </c>
-      <c r="G15" s="15">
-        <f t="shared" si="1"/>
+      <c r="G17" s="17">
+        <f>(F17-$F$4)/$F$4</f>
         <v>1.4995343896098711E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="18">
-      <c r="A16" s="3" t="s">
+      <c r="H17" s="13">
+        <v>1.30183920223378E-2</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1630524140732941E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="18">
+      <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B18" s="20">
         <v>0.28248171119676901</v>
       </c>
-      <c r="C16" s="15">
-        <f t="shared" si="2"/>
+      <c r="C18" s="17">
+        <f>(B18-$B$4)/$B$4</f>
         <v>1.9706319713551235E-3</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D18" s="13">
         <v>0.37988381547669597</v>
       </c>
-      <c r="E16" s="15">
-        <f t="shared" si="3"/>
+      <c r="E18" s="17">
+        <f>(D18-$D$4)/$D$4</f>
         <v>2.4173265794591534E-3</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F18" s="13">
         <v>0.53574071266044399</v>
       </c>
-      <c r="G16" s="15">
-        <f t="shared" si="1"/>
+      <c r="G18" s="17">
+        <f>(F18-$F$4)/$F$4</f>
         <v>2.2696711872948919E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="18">
-      <c r="A17" s="5" t="s">
+      <c r="H18" s="13">
+        <v>1.2860498542290801E-2</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="shared" si="0"/>
+        <v>-6.3902986442190184E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18">
+      <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B19" s="20">
         <v>0.29743571600449498</v>
       </c>
-      <c r="C17" s="15">
-        <f t="shared" si="2"/>
+      <c r="C19" s="17">
+        <f>(B19-$B$4)/$B$4</f>
         <v>5.501291065276253E-2</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D19" s="13">
         <v>0.39641490169830002</v>
       </c>
-      <c r="E17" s="15">
-        <f t="shared" si="3"/>
+      <c r="E19" s="17">
+        <f>(D19-$D$4)/$D$4</f>
         <v>4.6038682848403463E-2</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F19" s="13">
         <v>0.54917346358164898</v>
       </c>
-      <c r="G17" s="15">
-        <f t="shared" si="1"/>
+      <c r="G19" s="17">
+        <f>(F19-$F$4)/$F$4</f>
         <v>2.7399810694668961E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="18">
-      <c r="A18" s="5" t="s">
+      <c r="H19" s="13">
+        <v>1.22013399149368E-2</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" si="0"/>
+        <v>-5.1860792624202977E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18">
+      <c r="A20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B20" s="20">
         <v>0.28449176618636801</v>
       </c>
-      <c r="C18" s="15">
-        <f t="shared" si="2"/>
+      <c r="C20" s="17">
+        <f>(B20-$B$4)/$B$4</f>
         <v>9.1003539618268337E-3</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D20" s="13">
         <v>0.37848159362793099</v>
       </c>
-      <c r="E18" s="15">
-        <f t="shared" si="3"/>
+      <c r="E20" s="17">
+        <f>(D20-$D$4)/$D$4</f>
         <v>-1.282782295004148E-3</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F20" s="13">
         <v>0.53502293787451305</v>
       </c>
-      <c r="G18" s="15">
-        <f t="shared" si="1"/>
+      <c r="G20" s="17">
+        <f>(F20-$F$4)/$F$4</f>
         <v>9.268501515198996E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="18">
-      <c r="A19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="17">
-        <v>0.29268604756354599</v>
-      </c>
-      <c r="C19" s="15">
-        <f t="shared" si="2"/>
-        <v>3.8165702140502258E-2</v>
-      </c>
-      <c r="D19" s="10">
-        <v>0.37054064404786902</v>
-      </c>
-      <c r="E19" s="15">
-        <f t="shared" si="3"/>
-        <v>-2.2236940182881627E-2</v>
-      </c>
-      <c r="F19" s="10">
-        <v>0.53937298891714602</v>
-      </c>
-      <c r="G19" s="15">
-        <f t="shared" si="1"/>
-        <v>9.0649739213127124E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="18">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="17">
-        <v>0.29014039682978898</v>
-      </c>
-      <c r="C20" s="15">
-        <f t="shared" si="2"/>
-        <v>2.9136206872739136E-2</v>
-      </c>
-      <c r="D20" s="10">
-        <v>0.37869188174818902</v>
-      </c>
-      <c r="E20" s="15">
-        <f t="shared" si="3"/>
-        <v>-7.2788512188832132E-4</v>
-      </c>
-      <c r="F20" s="10">
-        <v>0.54993468130357903</v>
-      </c>
-      <c r="G20" s="15">
-        <f t="shared" si="1"/>
-        <v>2.8823905257264457E-2</v>
+      <c r="H20" s="13">
+        <v>1.28201992475918E-2</v>
+      </c>
+      <c r="I20" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.770599151081808E-3</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="18">
       <c r="A21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="17">
-        <v>0.29759868495102298</v>
-      </c>
-      <c r="C21" s="15">
-        <f t="shared" si="2"/>
-        <v>5.5590966122805445E-2</v>
-      </c>
-      <c r="D21" s="10">
-        <v>0.39726774857955199</v>
-      </c>
-      <c r="E21" s="15">
-        <f t="shared" si="3"/>
-        <v>4.8289130105845741E-2</v>
-      </c>
-      <c r="F21" s="10">
-        <v>0.546802537990702</v>
-      </c>
-      <c r="G21" s="15">
-        <f t="shared" si="1"/>
-        <v>2.2964256785302187E-2</v>
+        <v>28</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.29268604756354599</v>
+      </c>
+      <c r="C21" s="17">
+        <f>(B21-$B$4)/$B$4</f>
+        <v>3.8165702140502258E-2</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0.37054064404786902</v>
+      </c>
+      <c r="E21" s="17">
+        <f>(D21-$D$4)/$D$4</f>
+        <v>-2.2236940182881627E-2</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0.53937298891714602</v>
+      </c>
+      <c r="G21" s="17">
+        <f>(F21-$F$4)/$F$4</f>
+        <v>9.0649739213127124E-3</v>
+      </c>
+      <c r="H21" s="12">
+        <v>1.3648952584519701E-2</v>
+      </c>
+      <c r="I21" s="9">
+        <f t="shared" si="0"/>
+        <v>6.0629994346270678E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="18">
       <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.29014039682978898</v>
+      </c>
+      <c r="C22" s="17">
+        <f>(B22-$B$4)/$B$4</f>
+        <v>2.9136206872739136E-2</v>
+      </c>
+      <c r="D22" s="12">
+        <v>0.37869188174818902</v>
+      </c>
+      <c r="E22" s="17">
+        <f>(D22-$D$4)/$D$4</f>
+        <v>-7.2788512188832132E-4</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.54993468130357903</v>
+      </c>
+      <c r="G22" s="17">
+        <f>(F22-$F$4)/$F$4</f>
+        <v>2.8823905257264457E-2</v>
+      </c>
+      <c r="H22" s="12">
+        <v>1.1834066479690999E-2</v>
+      </c>
+      <c r="I22" s="9">
+        <f t="shared" si="0"/>
+        <v>-8.0400801034086158E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="18">
+      <c r="A23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0.29759868495102298</v>
+      </c>
+      <c r="C23" s="17">
+        <f>(B23-$B$4)/$B$4</f>
+        <v>5.5590966122805445E-2</v>
+      </c>
+      <c r="D23" s="12">
+        <v>0.39726774857955199</v>
+      </c>
+      <c r="E23" s="17">
+        <f>(D23-$D$4)/$D$4</f>
+        <v>4.8289130105845741E-2</v>
+      </c>
+      <c r="F23" s="12">
+        <v>0.546802537990702</v>
+      </c>
+      <c r="G23" s="17">
+        <f>(F23-$F$4)/$F$4</f>
+        <v>2.2964256785302187E-2</v>
+      </c>
+      <c r="H23" s="12">
+        <v>1.228505213996E-2</v>
+      </c>
+      <c r="I23" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.5355700295450184E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="18">
+      <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B24" s="19">
         <v>0.29107029321505701</v>
       </c>
-      <c r="C22" s="15">
-        <f t="shared" si="2"/>
+      <c r="C24" s="17">
+        <f>(B24-$B$4)/$B$4</f>
         <v>3.2434575694095732E-2</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D24" s="12">
         <v>0.39310991873477502</v>
       </c>
-      <c r="E22" s="15">
-        <f t="shared" si="3"/>
+      <c r="E24" s="17">
+        <f>(D24-$D$4)/$D$4</f>
         <v>3.7317668549518131E-2</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F24" s="12">
         <v>0.54872729136451703</v>
       </c>
-      <c r="G22" s="15">
-        <f t="shared" si="1"/>
+      <c r="G24" s="17">
+        <f>(F24-$F$4)/$F$4</f>
         <v>2.6565106758996312E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="18">
-      <c r="A23" s="5" t="s">
+      <c r="H24" s="12">
+        <v>1.23971755715701E-2</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="shared" si="0"/>
+        <v>-3.6642835780880539E-2</v>
+      </c>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" ht="18">
+      <c r="A25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B25" s="19">
         <v>0.29731305946279801</v>
       </c>
-      <c r="C23" s="15">
-        <f t="shared" si="2"/>
+      <c r="C25" s="17">
+        <f>(B25-$B$4)/$B$4</f>
         <v>5.4577844424655748E-2</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D25" s="12">
         <v>0.40030732402595998</v>
       </c>
-      <c r="E23" s="15">
-        <f t="shared" si="3"/>
+      <c r="E25" s="17">
+        <f>(D25-$D$4)/$D$4</f>
         <v>5.6309801081526646E-2</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F25" s="12">
         <v>0.54750841525724203</v>
       </c>
-      <c r="G23" s="15">
-        <f t="shared" si="1"/>
+      <c r="G25" s="17">
+        <f>(F25-$F$4)/$F$4</f>
         <v>2.4284819809755529E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="18">
-      <c r="A24" s="4" t="s">
+      <c r="H25" s="12">
+        <v>1.2269084034502799E-2</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="0"/>
+        <v>-4.6596546543242086E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="18">
+      <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B26" s="21">
         <v>0.28465564794916498</v>
       </c>
-      <c r="C24" s="16">
-        <f t="shared" si="2"/>
+      <c r="C26" s="18">
+        <f>(B26-$B$4)/$B$4</f>
         <v>9.6816472170347025E-3</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D26" s="14">
         <v>0.37587024242656902</v>
       </c>
-      <c r="E24" s="16">
-        <f t="shared" si="3"/>
+      <c r="E26" s="18">
+        <f>(D26-$D$4)/$D$4</f>
         <v>-8.1734777744747709E-3</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F26" s="14">
         <v>0.53622283927042402</v>
       </c>
-      <c r="G24" s="16">
-        <f t="shared" si="1"/>
+      <c r="G26" s="18">
+        <f>(F26-$F$4)/$F$4</f>
         <v>3.1716390001491797E-3</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:10" ht="18">
-      <c r="A25" s="53" t="s">
+      <c r="H26" s="14">
+        <v>1.31215634397718E-2</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9647747382744114E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18">
+      <c r="A27" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B27" s="26">
         <v>0.27991556719490701</v>
       </c>
-      <c r="C25" s="30">
-        <f t="shared" si="2"/>
+      <c r="C27" s="27">
+        <f>(B27-$B$4)/$B$4</f>
         <v>-7.1315534989252706E-3</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D27" s="63">
         <v>0.37430482179790697</v>
       </c>
-      <c r="E25" s="30">
-        <f t="shared" ref="E25" si="4">(D25-$D$3)/$D$3</f>
+      <c r="E27" s="27">
+        <f>(D27-$D$4)/$D$4</f>
         <v>-1.2304226960476913E-2</v>
       </c>
-      <c r="F25" s="65">
+      <c r="F27" s="63">
         <v>0.534854506675984</v>
       </c>
-      <c r="G25" s="30">
-        <f t="shared" si="1"/>
+      <c r="G27" s="27">
+        <f>(F27-$F$4)/$F$4</f>
         <v>6.1174719597060004E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="18">
-      <c r="A26" s="28" t="s">
+      <c r="H27" s="63">
+        <v>1.28609894062394E-2</v>
+      </c>
+      <c r="I27" s="78">
+        <f t="shared" si="0"/>
+        <v>-6.0088590987275863E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="18">
+      <c r="A28" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="29">
+      <c r="B28" s="26">
         <v>0.28416999852125602</v>
       </c>
-      <c r="C26" s="30">
-        <f t="shared" si="2"/>
+      <c r="C28" s="27">
+        <f>(B28-$B$4)/$B$4</f>
         <v>7.9590349383958422E-3</v>
       </c>
-      <c r="D26" s="65">
+      <c r="D28" s="63">
         <v>0.37040238377184798</v>
       </c>
-      <c r="E26" s="30">
-        <f t="shared" ref="E26" si="5">(D26-$D$3)/$D$3</f>
+      <c r="E28" s="27">
+        <f>(D28-$D$4)/$D$4</f>
         <v>-2.2601774088972716E-2</v>
       </c>
-      <c r="F26" s="65">
+      <c r="F28" s="63">
         <v>0.53200388355065997</v>
       </c>
-      <c r="G26" s="30">
-        <f t="shared" si="1"/>
+      <c r="G28" s="27">
+        <f>(F28-$F$4)/$F$4</f>
         <v>-4.7212301846531763E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="18">
-      <c r="A27" s="53" t="s">
+      <c r="H28" s="63">
+        <v>1.2637014260919901E-2</v>
+      </c>
+      <c r="I28" s="78">
+        <f t="shared" si="0"/>
+        <v>-1.8005500340386206E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="18">
+      <c r="A29" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="29">
+      <c r="B29" s="26">
         <v>0.27961524188424097</v>
       </c>
-      <c r="C27" s="30">
-        <f t="shared" si="2"/>
+      <c r="C29" s="27">
+        <f>(B29-$B$4)/$B$4</f>
         <v>-8.1968158837011605E-3</v>
       </c>
-      <c r="D27" s="65">
+      <c r="D29" s="63">
         <v>0.38296243580524197</v>
       </c>
-      <c r="E27" s="30">
-        <f t="shared" ref="E27" si="6">(D27-$D$3)/$D$3</f>
+      <c r="E29" s="27">
+        <f>(D29-$D$4)/$D$4</f>
         <v>1.0541027125695171E-2</v>
       </c>
-      <c r="F27" s="65">
+      <c r="F29" s="63">
         <v>0.53701945475882096</v>
       </c>
-      <c r="G27" s="30">
-        <f t="shared" si="1"/>
+      <c r="G29" s="27">
+        <f>(F29-$F$4)/$F$4</f>
         <v>4.6619560971146064E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="31" t="s">
+      <c r="H29" s="63">
+        <v>1.26458668330032E-2</v>
+      </c>
+      <c r="I29" s="78">
+        <f t="shared" si="0"/>
+        <v>-1.7317586493479829E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="18">
+      <c r="A30" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B30" s="26">
         <v>0.27201960930276498</v>
       </c>
-      <c r="C28" s="33">
-        <f t="shared" si="2"/>
+      <c r="C30" s="27">
+        <f>(B30-$B$4)/$B$4</f>
         <v>-3.5138739825043987E-2</v>
       </c>
-      <c r="D28" s="66">
+      <c r="D30" s="75">
         <v>0.36231217406210597</v>
       </c>
-      <c r="E28" s="33">
-        <f t="shared" ref="E28" si="7">(D28-$D$3)/$D$3</f>
+      <c r="E30" s="27">
+        <f>(D30-$D$4)/$D$4</f>
         <v>-4.394979171517837E-2</v>
       </c>
-      <c r="F28" s="66">
+      <c r="F30" s="75">
         <v>0.51233510855388997</v>
       </c>
-      <c r="G28" s="33">
-        <f t="shared" si="1"/>
+      <c r="G30" s="27">
+        <f>(F30-$F$4)/$F$4</f>
         <v>-4.1517792743384921E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="1" t="s">
+      <c r="H30" s="75">
+        <v>1.31626912160602E-2</v>
+      </c>
+      <c r="I30" s="78">
+        <f t="shared" si="0"/>
+        <v>2.2843696146000476E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="18">
+      <c r="A31" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="26">
+        <v>0.28090604176242401</v>
+      </c>
+      <c r="C31" s="27">
+        <f>(B31-$B$4)/$B$4</f>
+        <v>-3.6183121490268241E-3</v>
+      </c>
+      <c r="D31" s="63">
+        <v>0.36586808442567598</v>
+      </c>
+      <c r="E31" s="27">
+        <f>(D31-$D$4)/$D$4</f>
+        <v>-3.4566643460407033E-2</v>
+      </c>
+      <c r="F31" s="63">
+        <v>0.53275041973275306</v>
+      </c>
+      <c r="G31" s="27">
+        <f>(F31-$F$4)/$F$4</f>
+        <v>-3.3246020097284046E-3</v>
+      </c>
+      <c r="H31" s="63">
+        <v>1.2535645548559401E-2</v>
+      </c>
+      <c r="I31" s="78">
+        <f t="shared" si="0"/>
+        <v>-2.5882639348088966E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="18">
+      <c r="A32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="26">
+        <v>0.279331695298906</v>
+      </c>
+      <c r="C32" s="27">
+        <f>(B32-$B$4)/$B$4</f>
+        <v>-9.2025636544072788E-3</v>
+      </c>
+      <c r="D32" s="63">
+        <v>0.383255982113542</v>
+      </c>
+      <c r="E32" s="27">
+        <f>(D32-$D$4)/$D$4</f>
+        <v>1.1315621603283378E-2</v>
+      </c>
+      <c r="F32" s="63">
+        <v>0.53673611445874703</v>
+      </c>
+      <c r="G32" s="27">
+        <f>(F32-$F$4)/$F$4</f>
+        <v>4.1318799190713691E-3</v>
+      </c>
+      <c r="H32" s="63">
+        <v>1.29005175033796E-2</v>
+      </c>
+      <c r="I32" s="78">
+        <f t="shared" si="0"/>
+        <v>2.4707553158341881E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="18">
+      <c r="A33" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="26">
+        <v>0.281337130709434</v>
+      </c>
+      <c r="C33" s="27">
+        <f>(B33-$B$4)/$B$4</f>
+        <v>-2.0892274417673388E-3</v>
+      </c>
+      <c r="D33" s="63">
+        <v>0.39407782295149602</v>
+      </c>
+      <c r="E33" s="27">
+        <f>(D33-$D$4)/$D$4</f>
+        <v>3.9871723020338208E-2</v>
+      </c>
+      <c r="F33" s="63">
+        <v>0.52110962211769396</v>
+      </c>
+      <c r="G33" s="27">
+        <f>(F33-$F$4)/$F$4</f>
+        <v>-2.5102335383891228E-2</v>
+      </c>
+      <c r="H33" s="63">
+        <v>1.27824342656456E-2</v>
+      </c>
+      <c r="I33" s="78">
+        <f t="shared" si="0"/>
+        <v>-6.7052325846769069E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" ht="18">
+      <c r="A34" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="30">
+        <v>0.28192977099797001</v>
+      </c>
+      <c r="C34" s="31">
+        <f>(B34-$B$4)/$B$4</f>
+        <v>1.2884450433985989E-5</v>
+      </c>
+      <c r="D34" s="64">
+        <v>0.38089231436696802</v>
+      </c>
+      <c r="E34" s="31">
+        <f>(D34-$D$4)/$D$4</f>
+        <v>5.078500128472517E-3</v>
+      </c>
+      <c r="F34" s="64">
+        <v>0.53545832037546803</v>
+      </c>
+      <c r="G34" s="31">
+        <f>(F34-$F$4)/$F$4</f>
+        <v>1.7413685664185417E-3</v>
+      </c>
+      <c r="H34" s="64">
+        <v>1.2829323369105999E-2</v>
+      </c>
+      <c r="I34" s="78">
+        <f t="shared" si="0"/>
+        <v>-3.06158379696626E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" ht="18">
+      <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="54">
+      <c r="B35" s="52">
         <v>0.28204243536143497</v>
       </c>
-      <c r="C29" s="14">
-        <f t="shared" si="2"/>
+      <c r="C35" s="16">
+        <f>(B35-$B$4)/$B$4</f>
         <v>4.1250813928585565E-4</v>
       </c>
-      <c r="D29" s="67">
+      <c r="D35" s="65">
         <v>0.37621433965810802</v>
       </c>
-      <c r="E29" s="14">
-        <f t="shared" ref="E29" si="8">(D29-$D$3)/$D$3</f>
+      <c r="E35" s="16">
+        <f>(D35-$D$4)/$D$4</f>
         <v>-7.2654921934363105E-3</v>
       </c>
-      <c r="F29" s="67">
+      <c r="F35" s="65">
         <v>0.53516201806589503</v>
       </c>
-      <c r="G29" s="14">
-        <f t="shared" si="1"/>
+      <c r="G35" s="16">
+        <f>(F35-$F$4)/$F$4</f>
         <v>1.187042917144999E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="18">
-      <c r="A30" s="55" t="s">
+      <c r="H35" s="65">
+        <v>1.25949579398106E-2</v>
+      </c>
+      <c r="I35" s="79">
+        <f t="shared" si="0"/>
+        <v>-2.1273604273209158E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" ht="18">
+      <c r="A36" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="54">
+      <c r="B36" s="52">
         <v>0.28288709137675999</v>
       </c>
-      <c r="C30" s="14">
-        <f t="shared" si="2"/>
+      <c r="C36" s="16">
+        <f>(B36-$B$4)/$B$4</f>
         <v>3.4085269537006816E-3</v>
       </c>
-      <c r="D30" s="67">
+      <c r="D36" s="65">
         <v>0.38397906458662401</v>
       </c>
-      <c r="E30" s="14">
-        <f t="shared" ref="E30" si="9">(D30-$D$3)/$D$3</f>
+      <c r="E36" s="16">
+        <f>(D36-$D$4)/$D$4</f>
         <v>1.3223653401515621E-2</v>
       </c>
-      <c r="F30" s="67">
+      <c r="F36" s="65">
         <v>0.53220356093346799</v>
       </c>
-      <c r="G30" s="14">
-        <f t="shared" si="1"/>
+      <c r="G36" s="16">
+        <f>(F36-$F$4)/$F$4</f>
         <v>-4.3476715207676217E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="18">
-      <c r="A31" s="2" t="s">
+      <c r="H36" s="65">
+        <v>1.26793578824143E-2</v>
+      </c>
+      <c r="I36" s="79">
+        <f t="shared" si="0"/>
+        <v>-1.4715070928451514E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" ht="18">
+      <c r="A37" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="56">
+      <c r="B37" s="54">
         <v>0.28198685171297899</v>
       </c>
-      <c r="C31" s="20">
-        <f t="shared" si="2"/>
+      <c r="C37" s="22">
+        <f>(B37-$B$4)/$B$4</f>
         <v>2.1535136359668945E-4</v>
       </c>
-      <c r="D31" s="68">
+      <c r="D37" s="66">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E31" s="20">
-        <f t="shared" ref="E31" si="10">(D31-$D$3)/$D$3</f>
+      <c r="E37" s="22">
+        <f>(D37-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F31" s="68">
+      <c r="F37" s="66">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G31" s="20">
-        <f t="shared" si="1"/>
+      <c r="G37" s="22">
+        <f>(F37-$F$4)/$F$4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="18">
-      <c r="A32" s="34" t="s">
+      <c r="H37" s="66">
+        <v>1.2868722039991299E-2</v>
+      </c>
+      <c r="I37" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" ht="18">
+      <c r="A38" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="35">
+      <c r="B38" s="33">
         <v>0.28431155603143099</v>
       </c>
-      <c r="C32" s="36">
-        <f t="shared" si="2"/>
+      <c r="C38" s="34">
+        <f>(B38-$B$4)/$B$4</f>
         <v>8.4611434371351085E-3</v>
       </c>
-      <c r="D32" s="69">
+      <c r="D38" s="67">
         <v>0.37632945129837098</v>
       </c>
-      <c r="E32" s="36">
-        <f t="shared" ref="E32" si="11">(D32-$D$3)/$D$3</f>
+      <c r="E38" s="34">
+        <f>(D38-$D$4)/$D$4</f>
         <v>-6.9617416834395346E-3</v>
       </c>
-      <c r="F32" s="69">
+      <c r="F38" s="67">
         <v>0.53565031487291603</v>
       </c>
-      <c r="G32" s="36">
-        <f t="shared" si="1"/>
+      <c r="G38" s="34">
+        <f>(F38-$F$4)/$F$4</f>
         <v>2.1005540031037331E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="18">
-      <c r="A33" s="37" t="s">
+      <c r="H38" s="67">
+        <v>1.2602666476783E-2</v>
+      </c>
+      <c r="I38" s="80">
+        <f t="shared" si="0"/>
+        <v>-2.0674590870911277E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" ht="18">
+      <c r="A39" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="35">
+      <c r="B39" s="33">
         <v>0.28245202296716598</v>
       </c>
-      <c r="C33" s="36">
-        <f t="shared" si="2"/>
+      <c r="C39" s="34">
+        <f>(B39-$B$4)/$B$4</f>
         <v>1.8653269799224607E-3</v>
       </c>
-      <c r="D33" s="69">
+      <c r="D39" s="67">
         <v>0.38397906458662401</v>
       </c>
-      <c r="E33" s="36">
-        <f t="shared" ref="E33" si="12">(D33-$D$3)/$D$3</f>
+      <c r="E39" s="34">
+        <f>(D39-$D$4)/$D$4</f>
         <v>1.3223653401515621E-2</v>
       </c>
-      <c r="F33" s="69">
+      <c r="F39" s="67">
         <v>0.53229348457394998</v>
       </c>
-      <c r="G33" s="36">
-        <f t="shared" si="1"/>
+      <c r="G39" s="34">
+        <f>(F39-$F$4)/$F$4</f>
         <v>-4.1794413761323847E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="18">
-      <c r="A34" s="38" t="s">
+      <c r="H39" s="67">
+        <v>1.26848774356021E-2</v>
+      </c>
+      <c r="I39" s="80">
+        <f t="shared" si="0"/>
+        <v>-1.4286158626931025E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="18">
+      <c r="A40" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="39">
+      <c r="B40" s="37">
         <v>0.28198706819201902</v>
       </c>
-      <c r="C34" s="40">
-        <f t="shared" si="2"/>
+      <c r="C40" s="38">
+        <f>(B40-$B$4)/$B$4</f>
         <v>2.1611922088424852E-4</v>
       </c>
-      <c r="D34" s="70">
+      <c r="D40" s="68">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E34" s="40">
-        <f t="shared" ref="E34" si="13">(D34-$D$3)/$D$3</f>
+      <c r="E40" s="38">
+        <f>(D40-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F34" s="70">
+      <c r="F40" s="68">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G34" s="40">
-        <f t="shared" si="1"/>
+      <c r="G40" s="38">
+        <f>(F40-$F$4)/$F$4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="18">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="26"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
+      <c r="H40" s="68">
+        <v>1.2868722039991299E-2</v>
+      </c>
+      <c r="I40" s="80">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="82"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="72"/>
+      <c r="N40" s="72"/>
+      <c r="O40" s="72"/>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="J41" s="72"/>
+      <c r="K41" s="72"/>
+      <c r="L41" s="72"/>
+      <c r="M41" s="72"/>
+      <c r="N41" s="72"/>
+      <c r="O41" s="72"/>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="J42" s="72"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="74"/>
+      <c r="O42" s="74"/>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="J43" s="72"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="72"/>
+      <c r="O43" s="72"/>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="J44" s="72"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="74"/>
+      <c r="M44" s="74"/>
+      <c r="N44" s="74"/>
+      <c r="O44" s="74"/>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="72"/>
+      <c r="N45" s="72"/>
+      <c r="O45" s="72"/>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="J46" s="72"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="74"/>
+      <c r="M46" s="74"/>
+      <c r="N46" s="74"/>
+      <c r="O46" s="74"/>
+      <c r="T46" s="24"/>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="J47" s="72"/>
+      <c r="K47" s="72"/>
+      <c r="L47" s="72"/>
+      <c r="M47" s="72"/>
+      <c r="N47" s="72"/>
+      <c r="O47" s="72"/>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="J48" s="72"/>
+      <c r="K48" s="72"/>
+      <c r="L48" s="72"/>
+      <c r="M48" s="72"/>
+      <c r="N48" s="72"/>
+      <c r="O48" s="72"/>
+    </row>
+    <row r="49" spans="10:15" ht="18">
+      <c r="J49" s="72"/>
+      <c r="K49" s="73"/>
+      <c r="L49" s="72"/>
+      <c r="M49" s="72"/>
+      <c r="N49" s="72"/>
+      <c r="O49" s="72"/>
+    </row>
+    <row r="50" spans="10:15">
+      <c r="J50" s="72"/>
+      <c r="K50" s="72"/>
+      <c r="L50" s="72"/>
+      <c r="M50" s="72"/>
+      <c r="N50" s="72"/>
+      <c r="O50" s="72"/>
+    </row>
+    <row r="51" spans="10:15">
+      <c r="J51" s="72"/>
+      <c r="K51" s="72"/>
+      <c r="L51" s="72"/>
+      <c r="M51" s="72"/>
+      <c r="N51" s="72"/>
+      <c r="O51" s="72"/>
+    </row>
+    <row r="52" spans="10:15">
+      <c r="J52" s="72"/>
+      <c r="K52" s="72"/>
+      <c r="L52" s="72"/>
+      <c r="M52" s="72"/>
+      <c r="N52" s="72"/>
+      <c r="O52" s="72"/>
+    </row>
+    <row r="53" spans="10:15">
+      <c r="J53" s="72"/>
+      <c r="K53" s="72"/>
+      <c r="L53" s="72"/>
+      <c r="M53" s="72"/>
+      <c r="N53" s="72"/>
+      <c r="O53" s="72"/>
+    </row>
+    <row r="54" spans="10:15">
+      <c r="J54" s="72"/>
+      <c r="K54" s="72"/>
+      <c r="L54" s="72"/>
+      <c r="M54" s="72"/>
+      <c r="N54" s="72"/>
+      <c r="O54" s="72"/>
+    </row>
+    <row r="55" spans="10:15">
+      <c r="J55" s="72"/>
+      <c r="K55" s="72"/>
+      <c r="L55" s="72"/>
+      <c r="M55" s="72"/>
+      <c r="N55" s="72"/>
+      <c r="O55" s="72"/>
+    </row>
+    <row r="56" spans="10:15">
+      <c r="J56" s="72"/>
+      <c r="K56" s="72"/>
+      <c r="L56" s="72"/>
+      <c r="M56" s="72"/>
+      <c r="N56" s="72"/>
+      <c r="O56" s="72"/>
+    </row>
+    <row r="57" spans="10:15">
+      <c r="J57" s="72"/>
+      <c r="K57" s="72"/>
+      <c r="L57" s="72"/>
+      <c r="M57" s="72"/>
+      <c r="N57" s="72"/>
+      <c r="O57" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2141,18 +3914,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="12.5" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.83203125" customWidth="1"/>
@@ -2161,10 +3934,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="3" spans="1:9" ht="40">
       <c r="A3" s="6" t="s">
@@ -2203,22 +3976,22 @@
       <c r="C4" s="7">
         <v>225</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D4" s="71">
         <v>10.6488888888888</v>
       </c>
-      <c r="E4" s="73">
+      <c r="E4" s="71">
         <v>5.7777777777777697</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="71">
         <v>1.65777777777777</v>
       </c>
-      <c r="G4" s="73">
+      <c r="G4" s="71">
         <v>2.7466666666666599</v>
       </c>
-      <c r="H4" s="73">
+      <c r="H4" s="71">
         <v>0.266666666666666</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="71">
         <v>0.2</v>
       </c>
     </row>
@@ -2230,22 +4003,22 @@
       <c r="C5" s="7">
         <v>35</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="71">
         <v>9.0571428571428498</v>
       </c>
-      <c r="E5" s="73">
+      <c r="E5" s="71">
         <v>5.8571428571428497</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="71">
         <v>1.4</v>
       </c>
-      <c r="G5" s="73">
+      <c r="G5" s="71">
         <v>1.28571428571428</v>
       </c>
-      <c r="H5" s="73">
+      <c r="H5" s="71">
         <v>0.25714285714285701</v>
       </c>
-      <c r="I5" s="73">
+      <c r="I5" s="71">
         <v>0.25714285714285701</v>
       </c>
     </row>
@@ -2257,32 +4030,51 @@
       <c r="C6" s="7">
         <v>30</v>
       </c>
-      <c r="D6" s="73">
+      <c r="D6" s="71">
         <v>12.9</v>
       </c>
-      <c r="E6" s="73">
+      <c r="E6" s="71">
         <v>9</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="71">
         <v>1.1666666666666601</v>
       </c>
-      <c r="G6" s="73">
+      <c r="G6" s="71">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H6" s="73">
+      <c r="H6" s="71">
         <v>0.4</v>
       </c>
-      <c r="I6" s="73">
+      <c r="I6" s="71">
         <v>0.133333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="7">
+        <v>83</v>
+      </c>
+      <c r="D7" s="71">
+        <v>9.4578313253011999</v>
+      </c>
+      <c r="E7" s="71">
+        <v>5.7108433734939696</v>
+      </c>
+      <c r="F7" s="71">
+        <v>1.31325301204819</v>
+      </c>
+      <c r="G7" s="71">
+        <v>1.87951807228915</v>
+      </c>
+      <c r="H7" s="71">
+        <v>0.108433734939759</v>
+      </c>
+      <c r="I7" s="71">
+        <v>0.44578313253011997</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="7"/>
@@ -2340,97 +4132,137 @@
     <row r="12" spans="1:9">
       <c r="A12" s="7"/>
       <c r="B12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="72">
+        <v>54</v>
+      </c>
+      <c r="C12" s="70">
         <v>1400</v>
       </c>
-      <c r="D12" s="73">
+      <c r="D12" s="71">
         <v>94.532857142857097</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="71">
         <v>51.817142857142798</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="71">
         <v>17.350000000000001</v>
       </c>
-      <c r="G12" s="73">
+      <c r="G12" s="71">
         <v>19.844999999999999</v>
       </c>
-      <c r="H12" s="73">
+      <c r="H12" s="71">
         <v>2.66642857142857</v>
       </c>
-      <c r="I12" s="73">
+      <c r="I12" s="71">
         <v>2.8542857142857101</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="72">
-        <v>82</v>
-      </c>
-      <c r="D13" s="73">
-        <v>30.9268292682926</v>
-      </c>
-      <c r="E13" s="73">
-        <v>17.9634146341463</v>
-      </c>
-      <c r="F13" s="73">
-        <v>6.0487804878048701</v>
-      </c>
-      <c r="G13" s="73">
-        <v>5.2560975609755998</v>
-      </c>
-      <c r="H13" s="73">
-        <v>0.65853658536585302</v>
-      </c>
-      <c r="I13" s="73">
-        <v>1</v>
+        <v>55</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1400</v>
+      </c>
+      <c r="D13" s="71">
+        <v>86.567142857142798</v>
+      </c>
+      <c r="E13" s="71">
+        <v>46.804285714285697</v>
+      </c>
+      <c r="F13" s="71">
+        <v>16.847857142857102</v>
+      </c>
+      <c r="G13" s="71">
+        <v>17.642142857142801</v>
+      </c>
+      <c r="H13" s="71">
+        <v>2.5871428571428501</v>
+      </c>
+      <c r="I13" s="71">
+        <v>2.6857142857142802</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="7"/>
       <c r="B14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="72">
-        <v>1033</v>
-      </c>
-      <c r="D14" s="73">
-        <v>90.272023233300999</v>
-      </c>
-      <c r="E14" s="73">
-        <v>48.018393030009598</v>
-      </c>
-      <c r="F14" s="73">
-        <v>14.8257502420135</v>
-      </c>
-      <c r="G14" s="73">
-        <v>20.6379477250726</v>
-      </c>
-      <c r="H14" s="73">
-        <v>2.9961277831558499</v>
-      </c>
-      <c r="I14" s="73">
-        <v>3.7938044530493702</v>
+        <v>17</v>
+      </c>
+      <c r="C14" s="70">
+        <v>82</v>
+      </c>
+      <c r="D14" s="71">
+        <v>30.9268292682926</v>
+      </c>
+      <c r="E14" s="71">
+        <v>17.9634146341463</v>
+      </c>
+      <c r="F14" s="71">
+        <v>6.0487804878048701</v>
+      </c>
+      <c r="G14" s="71">
+        <v>5.2560975609755998</v>
+      </c>
+      <c r="H14" s="71">
+        <v>0.65853658536585302</v>
+      </c>
+      <c r="I14" s="71">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="70">
+        <v>1033</v>
+      </c>
+      <c r="D15" s="71">
+        <v>90.272023233300999</v>
+      </c>
+      <c r="E15" s="71">
+        <v>48.018393030009598</v>
+      </c>
+      <c r="F15" s="71">
+        <v>14.8257502420135</v>
+      </c>
+      <c r="G15" s="71">
+        <v>20.6379477250726</v>
+      </c>
+      <c r="H15" s="71">
+        <v>2.9961277831558499</v>
+      </c>
+      <c r="I15" s="71">
+        <v>3.7938044530493702</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="7">
+        <v>423</v>
+      </c>
+      <c r="D16" s="71">
+        <v>346.28132387706802</v>
+      </c>
+      <c r="E16" s="71">
+        <v>169.19385342789599</v>
+      </c>
+      <c r="F16" s="71">
+        <v>72.801418439716301</v>
+      </c>
+      <c r="G16" s="71">
+        <v>64.600472813238696</v>
+      </c>
+      <c r="H16" s="71">
+        <v>18.234042553191401</v>
+      </c>
+      <c r="I16" s="71">
+        <v>21.451536643025999</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="7"/>

</xml_diff>

<commit_message>
Set up round 2 experiments
</commit_message>
<xml_diff>
--- a/records.xlsx
+++ b/records.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-300" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MAP Scores - Cran" sheetId="5" r:id="rId1"/>
@@ -409,11 +409,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -790,7 +791,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -960,8 +961,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1104,39 +1139,6 @@
     <xf numFmtId="164" fontId="3" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1177,26 +1179,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="3" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1242,9 +1232,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1275,8 +1262,101 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="203">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1361,6 +1441,23 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1444,6 +1541,23 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -1777,7 +1891,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1794,25 +1908,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="74" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88" t="s">
+      <c r="C1" s="136"/>
+      <c r="D1" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88" t="s">
+      <c r="E1" s="136"/>
+      <c r="F1" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88" t="s">
+      <c r="G1" s="136"/>
+      <c r="H1" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="88"/>
+      <c r="I1" s="136"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1" thickBot="1">
       <c r="A2" s="5" t="s">
@@ -1847,31 +1961,31 @@
       <c r="A3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="41">
+      <c r="B3" s="107">
         <v>0.238436125225614</v>
       </c>
-      <c r="C3" s="91">
-        <f t="shared" ref="C3:C18" si="0">(B3-$B$4)/$B$4</f>
+      <c r="C3" s="76">
+        <f t="shared" ref="C3:C11" si="0">(B3-$B$4)/$B$4</f>
         <v>-2.2047539075231905E-2</v>
       </c>
-      <c r="D3" s="43">
+      <c r="D3" s="116">
         <v>0.377836663007103</v>
       </c>
-      <c r="E3" s="91">
-        <f t="shared" ref="E3:E18" si="1">(D3-$D$4)/$D$4</f>
+      <c r="E3" s="76">
+        <f t="shared" ref="E3:E11" si="1">(D3-$D$4)/$D$4</f>
         <v>-2.9845911176526658E-3</v>
       </c>
-      <c r="F3" s="43">
+      <c r="F3" s="116">
         <v>0.52990836804548702</v>
       </c>
-      <c r="G3" s="91">
-        <f t="shared" ref="G3:G18" si="2">(F3-$F$4)/$F$4</f>
+      <c r="G3" s="76">
+        <f t="shared" ref="G3:G11" si="2">(F3-$F$4)/$F$4</f>
         <v>-8.6415438489028037E-3</v>
       </c>
-      <c r="H3" s="43">
+      <c r="H3" s="116">
         <v>1.2091846347657E-2</v>
       </c>
-      <c r="I3" s="102">
+      <c r="I3" s="87">
         <f>(H3-$H$4)/$H$4</f>
         <v>-6.0369296183416854E-2</v>
       </c>
@@ -1880,31 +1994,31 @@
       <c r="A4" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="108">
         <v>0.24381157034989701</v>
       </c>
-      <c r="C4" s="92">
+      <c r="C4" s="77">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D4" s="33">
+      <c r="D4" s="117">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E4" s="92">
+      <c r="E4" s="77">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="117">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G4" s="92">
+      <c r="G4" s="77">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="117">
         <v>1.2868722039991299E-2</v>
       </c>
-      <c r="I4" s="102">
+      <c r="I4" s="87">
         <f>(H4-$H$4)/$H$4</f>
         <v>0</v>
       </c>
@@ -1916,31 +2030,31 @@
       <c r="A5" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="109">
         <v>0.243523296438478</v>
       </c>
-      <c r="C5" s="93">
+      <c r="C5" s="78">
         <f t="shared" si="0"/>
         <v>-1.1823635400292772E-3</v>
       </c>
-      <c r="D5" s="61">
+      <c r="D5" s="118">
         <v>0.38051722958994599</v>
       </c>
-      <c r="E5" s="94">
+      <c r="E5" s="79">
         <f t="shared" si="1"/>
         <v>4.0887462508263691E-3</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="119">
         <v>0.53245702655564198</v>
       </c>
-      <c r="G5" s="93">
+      <c r="G5" s="78">
         <f t="shared" si="2"/>
         <v>-3.8734852217050409E-3</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="119">
         <v>1.2836612529088401E-2</v>
       </c>
-      <c r="I5" s="103">
+      <c r="I5" s="88">
         <f t="shared" ref="I5:I11" si="3">(H5-$H$4)/$H$4</f>
         <v>-2.495159255372375E-3</v>
       </c>
@@ -1952,31 +2066,31 @@
       <c r="A6" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="109">
         <v>0.24364250981777499</v>
       </c>
-      <c r="C6" s="93">
+      <c r="C6" s="78">
         <f t="shared" si="0"/>
         <v>-6.9340651831818691E-4</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="118">
         <v>0.38075532482804098</v>
       </c>
-      <c r="E6" s="94">
+      <c r="E6" s="79">
         <f t="shared" si="1"/>
         <v>4.7170193762370322E-3</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="119">
         <v>0.53448952245516301</v>
       </c>
-      <c r="G6" s="93">
+      <c r="G6" s="78">
         <f t="shared" si="2"/>
         <v>-7.1069335134913222E-5</v>
       </c>
-      <c r="H6" s="37">
+      <c r="H6" s="119">
         <v>1.28553889656025E-2</v>
       </c>
-      <c r="I6" s="103">
+      <c r="I6" s="88">
         <f t="shared" si="3"/>
         <v>-1.0360837966167419E-3</v>
       </c>
@@ -1988,31 +2102,31 @@
       <c r="A7" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="109">
         <v>0.243809826790511</v>
       </c>
-      <c r="C7" s="93">
+      <c r="C7" s="78">
         <f t="shared" si="0"/>
         <v>-7.1512577664219435E-6</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="119">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E7" s="93">
+      <c r="E7" s="78">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F7" s="37">
+      <c r="F7" s="119">
         <v>0.53490309970692496</v>
       </c>
-      <c r="G7" s="93">
+      <c r="G7" s="78">
         <f t="shared" si="2"/>
         <v>7.0265557756685963E-4</v>
       </c>
-      <c r="H7" s="37">
+      <c r="H7" s="119">
         <v>1.28463878450113E-2</v>
       </c>
-      <c r="I7" s="103">
+      <c r="I7" s="88">
         <f t="shared" si="3"/>
         <v>-1.7355410203587589E-3</v>
       </c>
@@ -2024,31 +2138,31 @@
       <c r="A8" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="109">
         <v>0.243783355871317</v>
       </c>
-      <c r="C8" s="93">
+      <c r="C8" s="78">
         <f t="shared" si="0"/>
         <v>-1.1572247592481619E-4</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="119">
         <v>0.37890820290861998</v>
       </c>
-      <c r="E8" s="93">
+      <c r="E8" s="78">
         <f t="shared" si="1"/>
         <v>-1.5706828135072501E-4</v>
       </c>
-      <c r="F8" s="37">
+      <c r="F8" s="119">
         <v>0.53332300432032598</v>
       </c>
-      <c r="G8" s="93">
+      <c r="G8" s="78">
         <f t="shared" si="2"/>
         <v>-2.2534044084414613E-3</v>
       </c>
-      <c r="H8" s="37">
+      <c r="H8" s="119">
         <v>1.2852660847080401E-2</v>
       </c>
-      <c r="I8" s="103">
+      <c r="I8" s="88">
         <f t="shared" si="3"/>
         <v>-1.2480798684582845E-3</v>
       </c>
@@ -2060,31 +2174,31 @@
       <c r="A9" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="109">
         <v>0.24381987312621201</v>
       </c>
-      <c r="C9" s="93">
+      <c r="C9" s="78">
         <f t="shared" si="0"/>
         <v>3.4054070129176706E-5</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="119">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E9" s="93">
+      <c r="E9" s="78">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F9" s="37">
+      <c r="F9" s="119">
         <v>0.53464723638979195</v>
       </c>
-      <c r="G9" s="93">
+      <c r="G9" s="78">
         <f t="shared" si="2"/>
         <v>2.2398364416401637E-4</v>
       </c>
-      <c r="H9" s="37">
+      <c r="H9" s="119">
         <v>1.2868722039991299E-2</v>
       </c>
-      <c r="I9" s="103">
+      <c r="I9" s="88">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2096,31 +2210,31 @@
       <c r="A10" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="109">
         <v>0.243847179013993</v>
       </c>
-      <c r="C10" s="93">
+      <c r="C10" s="78">
         <f t="shared" si="0"/>
         <v>1.4604993538612837E-4</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="118">
         <v>0.38081484863756498</v>
       </c>
-      <c r="E10" s="94">
+      <c r="E10" s="79">
         <f t="shared" si="1"/>
         <v>4.8740876575903936E-3</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="119">
         <v>0.534374092550572</v>
       </c>
-      <c r="G10" s="93">
+      <c r="G10" s="78">
         <f t="shared" si="2"/>
         <v>-2.8701688174771311E-4</v>
       </c>
-      <c r="H10" s="37">
+      <c r="H10" s="119">
         <v>1.2866782451980301E-2</v>
       </c>
-      <c r="I10" s="103">
+      <c r="I10" s="88">
         <f t="shared" si="3"/>
         <v>-1.5072110540356279E-4</v>
       </c>
@@ -2129,64 +2243,64 @@
       <c r="A11" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="58">
+      <c r="B11" s="110">
         <v>0.24409659250321</v>
       </c>
-      <c r="C11" s="94">
+      <c r="C11" s="79">
         <f t="shared" si="0"/>
         <v>1.1690263628750606E-3</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="119">
         <v>0.37854437159783499</v>
       </c>
-      <c r="E11" s="93">
+      <c r="E11" s="78">
         <f t="shared" si="1"/>
         <v>-1.1171271072981633E-3</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="119">
         <v>0.53396353013215103</v>
       </c>
-      <c r="G11" s="93">
+      <c r="G11" s="78">
         <f t="shared" si="2"/>
         <v>-1.0551016107749277E-3</v>
       </c>
-      <c r="H11" s="37">
+      <c r="H11" s="119">
         <v>1.28505843180998E-2</v>
       </c>
-      <c r="I11" s="103">
+      <c r="I11" s="88">
         <f t="shared" si="3"/>
         <v>-1.4094423545037292E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="18">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="83">
+      <c r="B12" s="111">
         <v>0.24260216259627099</v>
       </c>
-      <c r="C12" s="95">
-        <f t="shared" si="0"/>
+      <c r="C12" s="80">
+        <f>(B12-$B$4)/$B$4</f>
         <v>-4.9604198516517584E-3</v>
       </c>
-      <c r="D12" s="84">
+      <c r="D12" s="120">
         <v>0.373911491596437</v>
       </c>
-      <c r="E12" s="95">
-        <f t="shared" si="1"/>
+      <c r="E12" s="80">
+        <f>(D12-$D$4)/$D$4</f>
         <v>-1.3342125899461012E-2</v>
       </c>
-      <c r="F12" s="84">
+      <c r="F12" s="120">
         <v>0.52623075858244905</v>
       </c>
-      <c r="G12" s="95">
-        <f t="shared" si="2"/>
+      <c r="G12" s="80">
+        <f>(F12-$F$4)/$F$4</f>
         <v>-1.5521656448466488E-2</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="134">
         <v>1.2890574020298799E-2</v>
       </c>
-      <c r="I12" s="104">
+      <c r="I12" s="89">
         <f t="shared" ref="I12:I18" si="4">(H12-$H$4)/$H$4</f>
         <v>1.6980691819740864E-3</v>
       </c>
@@ -2195,31 +2309,31 @@
       <c r="A13" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="109">
         <v>0.24422019593872701</v>
       </c>
-      <c r="C13" s="93">
-        <f t="shared" si="0"/>
+      <c r="C13" s="78">
+        <f>(B13-$B$4)/$B$4</f>
         <v>1.6759893234089944E-3</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="119">
         <v>0.37331535840631902</v>
       </c>
-      <c r="E13" s="93">
-        <f t="shared" si="1"/>
+      <c r="E13" s="78">
+        <f>(D13-$D$4)/$D$4</f>
         <v>-1.4915170642031794E-2</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="119">
         <v>0.52272475621146697</v>
       </c>
-      <c r="G13" s="93">
-        <f t="shared" si="2"/>
+      <c r="G13" s="78">
+        <f>(F13-$F$4)/$F$4</f>
         <v>-2.2080724595623082E-2</v>
       </c>
-      <c r="H13" s="61">
+      <c r="H13" s="118">
         <v>1.28998446009914E-2</v>
       </c>
-      <c r="I13" s="105">
+      <c r="I13" s="90">
         <f t="shared" si="4"/>
         <v>2.4184655557391564E-3</v>
       </c>
@@ -2228,31 +2342,31 @@
       <c r="A14" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="109">
         <v>0.24360166884019499</v>
       </c>
-      <c r="C14" s="93">
-        <f t="shared" si="0"/>
+      <c r="C14" s="78">
+        <f>(B14-$B$4)/$B$4</f>
         <v>-8.6091693433901803E-4</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D14" s="119">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E14" s="93">
-        <f t="shared" si="1"/>
+      <c r="E14" s="78">
+        <f>(D14-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="119">
         <v>0.53655180656797896</v>
       </c>
-      <c r="G14" s="93">
-        <f t="shared" si="2"/>
+      <c r="G14" s="78">
+        <f>(F14-$F$4)/$F$4</f>
         <v>3.7870746714731471E-3</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="119">
         <v>1.28607851541079E-2</v>
       </c>
-      <c r="I14" s="103">
+      <c r="I14" s="88">
         <f t="shared" si="4"/>
         <v>-6.1675789241035189E-4</v>
       </c>
@@ -2261,31 +2375,31 @@
       <c r="A15" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="109">
         <v>0.24237922459561601</v>
       </c>
-      <c r="C15" s="93">
-        <f t="shared" si="0"/>
+      <c r="C15" s="78">
+        <f>(B15-$B$4)/$B$4</f>
         <v>-5.8748063195910808E-3</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="119">
         <v>0.37658677433719101</v>
       </c>
-      <c r="E15" s="93">
-        <f t="shared" si="1"/>
+      <c r="E15" s="78">
+        <f>(D15-$D$4)/$D$4</f>
         <v>-6.2827312541123472E-3</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="119">
         <v>0.53504798095183503</v>
       </c>
-      <c r="G15" s="93">
-        <f t="shared" si="2"/>
+      <c r="G15" s="78">
+        <f>(F15-$F$4)/$F$4</f>
         <v>9.7370101851557611E-4</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H15" s="119">
         <v>1.28696643201362E-2</v>
       </c>
-      <c r="I15" s="103">
+      <c r="I15" s="88">
         <f t="shared" si="4"/>
         <v>7.3222511293069621E-5</v>
       </c>
@@ -2294,31 +2408,31 @@
       <c r="A16" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="109">
         <v>0.24381157034989701</v>
       </c>
-      <c r="C16" s="93">
-        <f t="shared" si="0"/>
+      <c r="C16" s="78">
+        <f>(B16-$B$4)/$B$4</f>
         <v>0</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="119">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E16" s="93">
-        <f t="shared" si="1"/>
+      <c r="E16" s="78">
+        <f>(D16-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F16" s="37">
+      <c r="F16" s="119">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G16" s="93">
-        <f t="shared" si="2"/>
+      <c r="G16" s="78">
+        <f>(F16-$F$4)/$F$4</f>
         <v>0</v>
       </c>
-      <c r="H16" s="37">
+      <c r="H16" s="119">
         <v>1.2868722039991299E-2</v>
       </c>
-      <c r="I16" s="103">
+      <c r="I16" s="88">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2327,31 +2441,31 @@
       <c r="A17" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="109">
         <v>0.24404322286174199</v>
       </c>
-      <c r="C17" s="93">
-        <f t="shared" si="0"/>
+      <c r="C17" s="78">
+        <f>(B17-$B$4)/$B$4</f>
         <v>9.5012928021641688E-4</v>
       </c>
-      <c r="D17" s="37">
+      <c r="D17" s="119">
         <v>0.374767477715581</v>
       </c>
-      <c r="E17" s="93">
-        <f t="shared" si="1"/>
+      <c r="E17" s="78">
+        <f>(D17-$D$4)/$D$4</f>
         <v>-1.1083394987051041E-2</v>
       </c>
-      <c r="F17" s="37">
+      <c r="F17" s="119">
         <v>0.53238225754980795</v>
       </c>
-      <c r="G17" s="93">
-        <f t="shared" si="2"/>
+      <c r="G17" s="78">
+        <f>(F17-$F$4)/$F$4</f>
         <v>-4.0133639076464821E-3</v>
       </c>
-      <c r="H17" s="61">
+      <c r="H17" s="118">
         <v>1.2905191395866799E-2</v>
       </c>
-      <c r="I17" s="105">
+      <c r="I17" s="90">
         <f t="shared" si="4"/>
         <v>2.83395318992566E-3</v>
       </c>
@@ -2360,64 +2474,64 @@
       <c r="A18" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="35">
+      <c r="B18" s="109">
         <v>0.24236669547370601</v>
       </c>
-      <c r="C18" s="93">
-        <f t="shared" si="0"/>
+      <c r="C18" s="78">
+        <f>(B18-$B$4)/$B$4</f>
         <v>-5.9261948648189075E-3</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="119">
         <v>0.374606645074199</v>
       </c>
-      <c r="E18" s="93">
-        <f t="shared" si="1"/>
+      <c r="E18" s="78">
+        <f>(D18-$D$4)/$D$4</f>
         <v>-1.1507791657381817E-2</v>
       </c>
-      <c r="F18" s="37">
+      <c r="F18" s="119">
         <v>0.53007490654408795</v>
       </c>
-      <c r="G18" s="93">
-        <f t="shared" si="2"/>
+      <c r="G18" s="78">
+        <f>(F18-$F$4)/$F$4</f>
         <v>-8.3299817773852432E-3</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="119">
         <v>1.2844000196088201E-2</v>
       </c>
-      <c r="I18" s="103">
+      <c r="I18" s="88">
         <f t="shared" si="4"/>
         <v>-1.921079950773051E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="112">
         <v>0.20670779224481001</v>
       </c>
-      <c r="C19" s="96">
+      <c r="C19" s="81">
         <f>(B19-$B$4)/$B$4</f>
         <v>-0.15218218746484799</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="121">
         <v>0.345222250131828</v>
       </c>
-      <c r="E19" s="96">
+      <c r="E19" s="81">
         <f>(D19-$D$4)/$D$4</f>
         <v>-8.904577938219306E-2</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="121">
         <v>0.49854150924888802</v>
       </c>
-      <c r="G19" s="96">
+      <c r="G19" s="81">
         <f>(F19-$F$4)/$F$4</f>
         <v>-6.7323011412058195E-2</v>
       </c>
-      <c r="H19" s="67">
+      <c r="H19" s="135">
         <v>1.380620281143E-2</v>
       </c>
-      <c r="I19" s="105">
+      <c r="I19" s="90">
         <f>(H19-$H$4)/$H$4</f>
         <v>7.2849562569255261E-2</v>
       </c>
@@ -2426,31 +2540,31 @@
       <c r="A20" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="108">
         <v>0.24353295067911801</v>
       </c>
-      <c r="C20" s="92">
+      <c r="C20" s="77">
         <f>(B20-$B$4)/$B$4</f>
         <v>-1.142766401033163E-3</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="122">
         <v>0.38526070879256302</v>
       </c>
-      <c r="E20" s="100">
+      <c r="E20" s="85">
         <f>(D20-$D$4)/$D$4</f>
         <v>1.6605588367424304E-2</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="117">
         <v>0.535015149771215</v>
       </c>
-      <c r="G20" s="92">
+      <c r="G20" s="77">
         <f>(F20-$F$4)/$F$4</f>
         <v>9.1228008143330532E-4</v>
       </c>
-      <c r="H20" s="33">
+      <c r="H20" s="117">
         <v>1.27313006966878E-2</v>
       </c>
-      <c r="I20" s="102">
+      <c r="I20" s="87">
         <f>(H20-$H$4)/$H$4</f>
         <v>-1.0678709422461952E-2</v>
       </c>
@@ -2459,31 +2573,31 @@
       <c r="A21" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="58">
+      <c r="B21" s="110">
         <v>0.25156069135867398</v>
       </c>
-      <c r="C21" s="97">
+      <c r="C21" s="82">
         <f>(B21-$B$4)/$B$4</f>
         <v>3.1783237348646402E-2</v>
       </c>
-      <c r="D21" s="61">
+      <c r="D21" s="118">
         <v>0.38577710973915302</v>
       </c>
-      <c r="E21" s="94">
+      <c r="E21" s="79">
         <f>(D21-$D$4)/$D$4</f>
         <v>1.7968239881478096E-2</v>
       </c>
-      <c r="F21" s="61">
+      <c r="F21" s="118">
         <v>0.55171276076341802</v>
       </c>
-      <c r="G21" s="94">
+      <c r="G21" s="79">
         <f>(F21-$F$4)/$F$4</f>
         <v>3.2150356044825232E-2</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="119">
         <v>1.23283812288041E-2</v>
       </c>
-      <c r="I21" s="103">
+      <c r="I21" s="88">
         <f>(H21-$H$4)/$H$4</f>
         <v>-4.1988692389812829E-2</v>
       </c>
@@ -2492,31 +2606,31 @@
       <c r="A22" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="59">
+      <c r="B22" s="113">
         <v>0.25046477420976698</v>
       </c>
-      <c r="C22" s="97">
+      <c r="C22" s="82">
         <f>(B22-$B$4)/$B$4</f>
         <v>2.7288302398126067E-2</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="123">
         <v>0.38163105961445798</v>
       </c>
-      <c r="E22" s="94">
+      <c r="E22" s="79">
         <f>(D22-$D$4)/$D$4</f>
         <v>7.0278620276703323E-3</v>
       </c>
-      <c r="F22" s="63">
+      <c r="F22" s="123">
         <v>0.54979644038339803</v>
       </c>
-      <c r="G22" s="94">
+      <c r="G22" s="79">
         <f>(F22-$F$4)/$F$4</f>
         <v>2.8565282609516841E-2</v>
       </c>
-      <c r="H22" s="46">
+      <c r="H22" s="124">
         <v>1.23842288253881E-2</v>
       </c>
-      <c r="I22" s="103">
+      <c r="I22" s="88">
         <f>(H22-$H$4)/$H$4</f>
         <v>-3.7648898864826703E-2</v>
       </c>
@@ -2525,31 +2639,31 @@
       <c r="A23" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="59">
+      <c r="B23" s="113">
         <v>0.247419697024271</v>
       </c>
-      <c r="C23" s="97">
+      <c r="C23" s="82">
         <f>(B23-$B$4)/$B$4</f>
         <v>1.4798832841263125E-2</v>
       </c>
-      <c r="D23" s="63">
+      <c r="D23" s="123">
         <v>0.37958748394504299</v>
       </c>
-      <c r="E23" s="94">
+      <c r="E23" s="79">
         <f>(D23-$D$4)/$D$4</f>
         <v>1.6353826017510493E-3</v>
       </c>
-      <c r="F23" s="63">
+      <c r="F23" s="123">
         <v>0.53844146954574501</v>
       </c>
-      <c r="G23" s="94">
+      <c r="G23" s="79">
         <f>(F23-$F$4)/$F$4</f>
         <v>7.3222771427865077E-3</v>
       </c>
-      <c r="H23" s="63">
+      <c r="H23" s="123">
         <v>1.3659904037220699E-2</v>
       </c>
-      <c r="I23" s="105">
+      <c r="I23" s="90">
         <f>(H23-$H$4)/$H$4</f>
         <v>6.1481007575631408E-2</v>
       </c>
@@ -2558,31 +2672,31 @@
       <c r="A24" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="59">
+      <c r="B24" s="113">
         <v>0.245402577321679</v>
       </c>
-      <c r="C24" s="97">
+      <c r="C24" s="82">
         <f>(B24-$B$4)/$B$4</f>
         <v>6.5255597570645241E-3</v>
       </c>
-      <c r="D24" s="46">
+      <c r="D24" s="124">
         <v>0.37669056162282799</v>
       </c>
-      <c r="E24" s="93">
+      <c r="E24" s="78">
         <f>(D24-$D$4)/$D$4</f>
         <v>-6.008862852346906E-3</v>
       </c>
-      <c r="F24" s="63">
+      <c r="F24" s="123">
         <v>0.53532905335487102</v>
       </c>
-      <c r="G24" s="94">
+      <c r="G24" s="79">
         <f>(F24-$F$4)/$F$4</f>
         <v>1.4995343896098711E-3</v>
       </c>
-      <c r="H24" s="63">
+      <c r="H24" s="123">
         <v>1.30183920223378E-2</v>
       </c>
-      <c r="I24" s="105">
+      <c r="I24" s="90">
         <f>(H24-$H$4)/$H$4</f>
         <v>1.1630524140732941E-2</v>
       </c>
@@ -2591,31 +2705,31 @@
       <c r="A25" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="59">
+      <c r="B25" s="113">
         <v>0.24552897807379301</v>
       </c>
-      <c r="C25" s="97">
+      <c r="C25" s="82">
         <f>(B25-$B$4)/$B$4</f>
         <v>7.0439959901465289E-3</v>
       </c>
-      <c r="D25" s="46">
+      <c r="D25" s="124">
         <v>0.37837587896875902</v>
       </c>
-      <c r="E25" s="93">
+      <c r="E25" s="78">
         <f>(D25-$D$4)/$D$4</f>
         <v>-1.5617365481471841E-3</v>
       </c>
-      <c r="F25" s="46">
+      <c r="F25" s="124">
         <v>0.53461485482603999</v>
       </c>
-      <c r="G25" s="93">
+      <c r="G25" s="78">
         <f>(F25-$F$4)/$F$4</f>
         <v>1.6340385530862398E-4</v>
       </c>
-      <c r="H25" s="63">
+      <c r="H25" s="123">
         <v>1.29112613523452E-2</v>
       </c>
-      <c r="I25" s="105">
+      <c r="I25" s="90">
         <f>(H25-$H$4)/$H$4</f>
         <v>3.3056361169123217E-3</v>
       </c>
@@ -2624,31 +2738,31 @@
       <c r="A26" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="59">
+      <c r="B26" s="113">
         <v>0.25372541704894802</v>
       </c>
-      <c r="C26" s="97">
+      <c r="C26" s="82">
         <f>(B26-$B$4)/$B$4</f>
         <v>4.0661920534876717E-2</v>
       </c>
-      <c r="D26" s="63">
+      <c r="D26" s="123">
         <v>0.40717684380385399</v>
       </c>
-      <c r="E26" s="94">
+      <c r="E26" s="79">
         <f>(D26-$D$4)/$D$4</f>
         <v>7.4436726657443081E-2</v>
       </c>
-      <c r="F26" s="63">
+      <c r="F26" s="123">
         <v>0.53771019706241896</v>
       </c>
-      <c r="G26" s="94">
+      <c r="G26" s="79">
         <f>(F26-$F$4)/$F$4</f>
         <v>5.9542044649199388E-3</v>
       </c>
-      <c r="H26" s="46">
+      <c r="H26" s="124">
         <v>1.27354253992739E-2</v>
       </c>
-      <c r="I26" s="103">
+      <c r="I26" s="88">
         <f>(H26-$H$4)/$H$4</f>
         <v>-1.035818788401534E-2</v>
       </c>
@@ -2657,31 +2771,31 @@
       <c r="A27" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="59">
+      <c r="B27" s="113">
         <v>0.24672743114774001</v>
       </c>
-      <c r="C27" s="97">
+      <c r="C27" s="82">
         <f>(B27-$B$4)/$B$4</f>
         <v>1.1959484915578118E-2</v>
       </c>
-      <c r="D27" s="46">
+      <c r="D27" s="124">
         <v>0.37670924469414202</v>
       </c>
-      <c r="E27" s="93">
+      <c r="E27" s="78">
         <f>(D27-$D$4)/$D$4</f>
         <v>-5.9595629515985637E-3</v>
       </c>
-      <c r="F27" s="63">
+      <c r="F27" s="123">
         <v>0.53620201130682799</v>
       </c>
-      <c r="G27" s="94">
+      <c r="G27" s="79">
         <f>(F27-$F$4)/$F$4</f>
         <v>3.1326738146936323E-3</v>
       </c>
-      <c r="H27" s="63">
+      <c r="H27" s="123">
         <v>1.31053301456072E-2</v>
       </c>
-      <c r="I27" s="105">
+      <c r="I27" s="90">
         <f>(H27-$H$4)/$H$4</f>
         <v>1.8386293905533816E-2</v>
       </c>
@@ -2690,31 +2804,31 @@
       <c r="A28" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="58">
+      <c r="B28" s="110">
         <v>0.24820233481440501</v>
       </c>
-      <c r="C28" s="94">
+      <c r="C28" s="79">
         <f>(B28-$B$4)/$B$4</f>
         <v>1.8008843707485934E-2</v>
       </c>
-      <c r="D28" s="37">
+      <c r="D28" s="119">
         <v>0.37054064404786902</v>
       </c>
-      <c r="E28" s="93">
+      <c r="E28" s="78">
         <f>(D28-$D$4)/$D$4</f>
         <v>-2.2236940182881627E-2</v>
       </c>
-      <c r="F28" s="61">
+      <c r="F28" s="118">
         <v>0.53937298891714602</v>
       </c>
-      <c r="G28" s="94">
+      <c r="G28" s="79">
         <f>(F28-$F$4)/$F$4</f>
         <v>9.0649739213127124E-3</v>
       </c>
-      <c r="H28" s="61">
+      <c r="H28" s="118">
         <v>1.3648952584519701E-2</v>
       </c>
-      <c r="I28" s="105">
+      <c r="I28" s="90">
         <f>(H28-$H$4)/$H$4</f>
         <v>6.0629994346270678E-2</v>
       </c>
@@ -2723,31 +2837,31 @@
       <c r="A29" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="58">
+      <c r="B29" s="110">
         <v>0.24699614031921799</v>
       </c>
-      <c r="C29" s="97">
+      <c r="C29" s="82">
         <f>(B29-$B$4)/$B$4</f>
         <v>1.3061603125523399E-2</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D29" s="119">
         <v>0.37160270863094502</v>
       </c>
-      <c r="E29" s="93">
+      <c r="E29" s="78">
         <f>(D29-$D$4)/$D$4</f>
         <v>-1.9434420315890644E-2</v>
       </c>
-      <c r="F29" s="61">
+      <c r="F29" s="118">
         <v>0.55361738190463805</v>
       </c>
-      <c r="G29" s="94">
+      <c r="G29" s="79">
         <f>(F29-$F$4)/$F$4</f>
         <v>3.5713542414342145E-2</v>
       </c>
-      <c r="H29" s="37">
+      <c r="H29" s="119">
         <v>1.2532039005573301E-2</v>
       </c>
-      <c r="I29" s="103">
+      <c r="I29" s="88">
         <f>(H29-$H$4)/$H$4</f>
         <v>-2.6162895847133116E-2</v>
       </c>
@@ -2756,31 +2870,31 @@
       <c r="A30" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="58">
+      <c r="B30" s="110">
         <v>0.25281148825765098</v>
       </c>
-      <c r="C30" s="97">
+      <c r="C30" s="82">
         <f>(B30-$B$4)/$B$4</f>
         <v>3.6913415941819683E-2</v>
       </c>
-      <c r="D30" s="61">
+      <c r="D30" s="118">
         <v>0.39972514736072501</v>
       </c>
-      <c r="E30" s="94">
+      <c r="E30" s="79">
         <f>(D30-$D$4)/$D$4</f>
         <v>5.4773584078889999E-2</v>
       </c>
-      <c r="F30" s="61">
+      <c r="F30" s="118">
         <v>0.53745433398489695</v>
       </c>
-      <c r="G30" s="94">
+      <c r="G30" s="79">
         <f>(F30-$F$4)/$F$4</f>
         <v>5.4755329797840091E-3</v>
       </c>
-      <c r="H30" s="37">
+      <c r="H30" s="119">
         <v>1.2860510696370101E-2</v>
       </c>
-      <c r="I30" s="103">
+      <c r="I30" s="88">
         <f>(H30-$H$4)/$H$4</f>
         <v>-6.3808539773262856E-4</v>
       </c>
@@ -2789,31 +2903,31 @@
       <c r="A31" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="B31" s="58">
+      <c r="B31" s="110">
         <v>0.251392039102381</v>
       </c>
-      <c r="C31" s="97">
+      <c r="C31" s="82">
         <f>(B31-$B$4)/$B$4</f>
         <v>3.1091505385102004E-2</v>
       </c>
-      <c r="D31" s="61">
+      <c r="D31" s="118">
         <v>0.387790674991634</v>
       </c>
-      <c r="E31" s="94">
+      <c r="E31" s="79">
         <f>(D31-$D$4)/$D$4</f>
         <v>2.3281529405940856E-2</v>
       </c>
-      <c r="F31" s="61">
+      <c r="F31" s="118">
         <v>0.55131885421681903</v>
       </c>
-      <c r="G31" s="94">
+      <c r="G31" s="79">
         <f>(F31-$F$4)/$F$4</f>
         <v>3.1413431305658518E-2</v>
       </c>
-      <c r="H31" s="37">
+      <c r="H31" s="119">
         <v>1.2243544156512401E-2</v>
       </c>
-      <c r="I31" s="103">
+      <c r="I31" s="88">
         <f>(H31-$H$4)/$H$4</f>
         <v>-4.8581194118271706E-2</v>
       </c>
@@ -2822,31 +2936,31 @@
       <c r="A32" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="58">
+      <c r="B32" s="110">
         <v>0.25303892731352501</v>
       </c>
-      <c r="C32" s="97">
+      <c r="C32" s="82">
         <f>(B32-$B$4)/$B$4</f>
         <v>3.7846263614092261E-2</v>
       </c>
-      <c r="D32" s="61">
+      <c r="D32" s="118">
         <v>0.40465041839565502</v>
       </c>
-      <c r="E32" s="94">
+      <c r="E32" s="79">
         <f>(D32-$D$4)/$D$4</f>
         <v>6.7770128870666371E-2</v>
       </c>
-      <c r="F32" s="61">
+      <c r="F32" s="118">
         <v>0.53777070538758698</v>
       </c>
-      <c r="G32" s="94">
+      <c r="G32" s="79">
         <f>(F32-$F$4)/$F$4</f>
         <v>6.0674041111986061E-3</v>
       </c>
-      <c r="H32" s="37">
+      <c r="H32" s="119">
         <v>1.28078215399848E-2</v>
       </c>
-      <c r="I32" s="103">
+      <c r="I32" s="88">
         <f>(H32-$H$4)/$H$4</f>
         <v>-4.7324435027225184E-3</v>
       </c>
@@ -2855,31 +2969,31 @@
       <c r="A33" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="60">
+      <c r="B33" s="114">
         <v>0.246826309053788</v>
       </c>
-      <c r="C33" s="98">
+      <c r="C33" s="83">
         <f>(B33-$B$4)/$B$4</f>
         <v>1.236503542290672E-2</v>
       </c>
-      <c r="D33" s="51">
+      <c r="D33" s="125">
         <v>0.37587024242656902</v>
       </c>
-      <c r="E33" s="101">
+      <c r="E33" s="86">
         <f>(D33-$D$4)/$D$4</f>
         <v>-8.1734777744747709E-3</v>
       </c>
-      <c r="F33" s="64">
+      <c r="F33" s="133">
         <v>0.53622283927042402</v>
       </c>
-      <c r="G33" s="100">
+      <c r="G33" s="85">
         <f>(F33-$F$4)/$F$4</f>
         <v>3.1716390001491797E-3</v>
       </c>
-      <c r="H33" s="64">
+      <c r="H33" s="133">
         <v>1.31215634397718E-2</v>
       </c>
-      <c r="I33" s="105">
+      <c r="I33" s="90">
         <f>(H33-$H$4)/$H$4</f>
         <v>1.9647747382744114E-2</v>
       </c>
@@ -2888,31 +3002,31 @@
       <c r="A34" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="58">
+      <c r="B34" s="110">
         <v>0.25007608223879102</v>
       </c>
-      <c r="C34" s="94">
+      <c r="C34" s="79">
         <f>(B34-$B$4)/$B$4</f>
         <v>2.5694071367916363E-2</v>
       </c>
-      <c r="D34" s="65">
+      <c r="D34" s="126">
         <v>0.37990998365474299</v>
       </c>
-      <c r="E34" s="94">
+      <c r="E34" s="79">
         <f>(D34-$D$4)/$D$4</f>
         <v>2.48637778409241E-3</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="127">
         <v>0.530784976806144</v>
       </c>
-      <c r="G34" s="99">
+      <c r="G34" s="84">
         <f>(F34-$F$4)/$F$4</f>
         <v>-7.0015744503843878E-3</v>
       </c>
-      <c r="H34" s="65">
+      <c r="H34" s="126">
         <v>1.30627044657086E-2</v>
       </c>
-      <c r="I34" s="105">
+      <c r="I34" s="90">
         <f>(H34-$H$4)/$H$4</f>
         <v>1.5073946357258615E-2</v>
       </c>
@@ -2921,31 +3035,31 @@
       <c r="A35" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="58">
+      <c r="B35" s="110">
         <v>0.24672868674183199</v>
       </c>
-      <c r="C35" s="94">
+      <c r="C35" s="79">
         <f>(B35-$B$4)/$B$4</f>
         <v>1.196463476999304E-2</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="127">
         <v>0.37040238377184798</v>
       </c>
-      <c r="E35" s="99">
+      <c r="E35" s="84">
         <f>(D35-$D$4)/$D$4</f>
         <v>-2.2601774088972716E-2</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="127">
         <v>0.53200388355065997</v>
       </c>
-      <c r="G35" s="99">
+      <c r="G35" s="84">
         <f>(F35-$F$4)/$F$4</f>
         <v>-4.7212301846531763E-3</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="127">
         <v>1.2637014260919901E-2</v>
       </c>
-      <c r="I35" s="102">
+      <c r="I35" s="87">
         <f>(H35-$H$4)/$H$4</f>
         <v>-1.8005500340386206E-2</v>
       </c>
@@ -2954,31 +3068,31 @@
       <c r="A36" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36" s="115">
         <v>0.24181080359844601</v>
       </c>
-      <c r="C36" s="99">
+      <c r="C36" s="84">
         <f>(B36-$B$4)/$B$4</f>
         <v>-8.2062009960383528E-3</v>
       </c>
-      <c r="D36" s="65">
+      <c r="D36" s="126">
         <v>0.38296243580524197</v>
       </c>
-      <c r="E36" s="94">
+      <c r="E36" s="79">
         <f>(D36-$D$4)/$D$4</f>
         <v>1.0541027125695171E-2</v>
       </c>
-      <c r="F36" s="65">
+      <c r="F36" s="126">
         <v>0.53701945475882096</v>
       </c>
-      <c r="G36" s="94">
+      <c r="G36" s="79">
         <f>(F36-$F$4)/$F$4</f>
         <v>4.6619560971146064E-3</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="127">
         <v>1.26458668330032E-2</v>
       </c>
-      <c r="I36" s="102">
+      <c r="I36" s="87">
         <f>(H36-$H$4)/$H$4</f>
         <v>-1.7317586493479829E-2</v>
       </c>
@@ -2987,31 +3101,31 @@
       <c r="A37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="115">
         <v>0.24376309399194701</v>
       </c>
-      <c r="C37" s="99">
+      <c r="C37" s="84">
         <f>(B37-$B$4)/$B$4</f>
         <v>-1.9882714294660299E-4</v>
       </c>
-      <c r="D37" s="23">
+      <c r="D37" s="128">
         <v>0.37466821983405002</v>
       </c>
-      <c r="E37" s="99">
+      <c r="E37" s="84">
         <f>(D37-$D$4)/$D$4</f>
         <v>-1.1345311436745983E-2</v>
       </c>
-      <c r="F37" s="23">
+      <c r="F37" s="128">
         <v>0.52984253599575704</v>
       </c>
-      <c r="G37" s="99">
+      <c r="G37" s="84">
         <f>(F37-$F$4)/$F$4</f>
         <v>-8.7647031781775946E-3</v>
       </c>
-      <c r="H37" s="68">
+      <c r="H37" s="123">
         <v>1.2942325244435801E-2</v>
       </c>
-      <c r="I37" s="105">
+      <c r="I37" s="90">
         <f>(H37-$H$4)/$H$4</f>
         <v>5.7195426411239224E-3</v>
       </c>
@@ -3020,31 +3134,31 @@
       <c r="A38" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="115">
         <v>0.24111532348086101</v>
       </c>
-      <c r="C38" s="99">
+      <c r="C38" s="84">
         <f>(B38-$B$4)/$B$4</f>
         <v>-1.1058732221635659E-2</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="127">
         <v>0.36586808442567598</v>
       </c>
-      <c r="E38" s="99">
+      <c r="E38" s="84">
         <f>(D38-$D$4)/$D$4</f>
         <v>-3.4566643460407033E-2</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="127">
         <v>0.53275041973275306</v>
       </c>
-      <c r="G38" s="99">
+      <c r="G38" s="84">
         <f>(F38-$F$4)/$F$4</f>
         <v>-3.3246020097284046E-3</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38" s="127">
         <v>1.2535645548559401E-2</v>
       </c>
-      <c r="I38" s="102">
+      <c r="I38" s="87">
         <f>(H38-$H$4)/$H$4</f>
         <v>-2.5882639348088966E-2</v>
       </c>
@@ -3053,31 +3167,31 @@
       <c r="A39" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="115">
         <v>0.24351461914792599</v>
       </c>
-      <c r="C39" s="99">
+      <c r="C39" s="84">
         <f>(B39-$B$4)/$B$4</f>
         <v>-1.217953690814815E-3</v>
       </c>
-      <c r="D39" s="65">
+      <c r="D39" s="126">
         <v>0.383255982113542</v>
       </c>
-      <c r="E39" s="94">
+      <c r="E39" s="79">
         <f>(D39-$D$4)/$D$4</f>
         <v>1.1315621603283378E-2</v>
       </c>
-      <c r="F39" s="65">
+      <c r="F39" s="126">
         <v>0.53673611445874703</v>
       </c>
-      <c r="G39" s="94">
+      <c r="G39" s="79">
         <f>(F39-$F$4)/$F$4</f>
         <v>4.1318799190713691E-3</v>
       </c>
-      <c r="H39" s="65">
+      <c r="H39" s="126">
         <v>1.29005175033796E-2</v>
       </c>
-      <c r="I39" s="105">
+      <c r="I39" s="90">
         <f>(H39-$H$4)/$H$4</f>
         <v>2.4707553158341881E-3</v>
       </c>
@@ -3086,31 +3200,31 @@
       <c r="A40" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B40" s="58">
+      <c r="B40" s="110">
         <v>0.24520815990716899</v>
       </c>
-      <c r="C40" s="94">
+      <c r="C40" s="79">
         <f>(B40-$B$4)/$B$4</f>
         <v>5.728151273820677E-3</v>
       </c>
-      <c r="D40" s="65">
+      <c r="D40" s="126">
         <v>0.38569019697707702</v>
       </c>
-      <c r="E40" s="94">
+      <c r="E40" s="79">
         <f>(D40-$D$4)/$D$4</f>
         <v>1.7738899080274068E-2</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="127">
         <v>0.52763862444377996</v>
       </c>
-      <c r="G40" s="99">
+      <c r="G40" s="84">
         <f>(F40-$F$4)/$F$4</f>
         <v>-1.288780536982673E-2</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="127">
         <v>1.27530290080649E-2</v>
       </c>
-      <c r="I40" s="102">
+      <c r="I40" s="87">
         <f>(H40-$H$4)/$H$4</f>
         <v>-8.9902502802428463E-3</v>
       </c>
@@ -3119,31 +3233,31 @@
       <c r="A41" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="60">
+      <c r="B41" s="114">
         <v>0.244667452224793</v>
       </c>
-      <c r="C41" s="100">
+      <c r="C41" s="85">
         <f>(B41-$B$4)/$B$4</f>
         <v>3.5104235359614193E-3</v>
       </c>
-      <c r="D41" s="66">
+      <c r="D41" s="129">
         <v>0.38177963590090602</v>
       </c>
-      <c r="E41" s="100">
+      <c r="E41" s="85">
         <f>(D41-$D$4)/$D$4</f>
         <v>7.4199172766349674E-3</v>
       </c>
-      <c r="F41" s="66">
+      <c r="F41" s="129">
         <v>0.53518687828056299</v>
       </c>
-      <c r="G41" s="100">
+      <c r="G41" s="85">
         <f>(F41-$F$4)/$F$4</f>
         <v>1.2335516826580274E-3</v>
       </c>
-      <c r="H41" s="16">
+      <c r="H41" s="132">
         <v>1.2782683254098299E-2</v>
       </c>
-      <c r="I41" s="102">
+      <c r="I41" s="87">
         <f>(H41-$H$4)/$H$4</f>
         <v>-6.6858842413118312E-3</v>
       </c>
@@ -3152,31 +3266,31 @@
       <c r="A42" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="35">
+      <c r="B42" s="109">
         <v>0.242987098680572</v>
       </c>
-      <c r="C42" s="93">
+      <c r="C42" s="78">
         <f>(B42-$B$4)/$B$4</f>
         <v>-3.3815936960735534E-3</v>
       </c>
-      <c r="D42" s="52">
+      <c r="D42" s="130">
         <v>0.37621433965810802</v>
       </c>
-      <c r="E42" s="93">
+      <c r="E42" s="78">
         <f>(D42-$D$4)/$D$4</f>
         <v>-7.2654921934363105E-3</v>
       </c>
-      <c r="F42" s="65">
+      <c r="F42" s="126">
         <v>0.53516201806589503</v>
       </c>
-      <c r="G42" s="94">
+      <c r="G42" s="79">
         <f>(F42-$F$4)/$F$4</f>
         <v>1.187042917144999E-3</v>
       </c>
-      <c r="H42" s="52">
+      <c r="H42" s="130">
         <v>1.25949579398106E-2</v>
       </c>
-      <c r="I42" s="103">
+      <c r="I42" s="88">
         <f>(H42-$H$4)/$H$4</f>
         <v>-2.1273604273209158E-2</v>
       </c>
@@ -3185,31 +3299,31 @@
       <c r="A43" s="53" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="58">
+      <c r="B43" s="110">
         <v>0.245066169139806</v>
       </c>
-      <c r="C43" s="97">
+      <c r="C43" s="82">
         <f>(B43-$B$4)/$B$4</f>
         <v>5.1457721555564599E-3</v>
       </c>
-      <c r="D43" s="65">
+      <c r="D43" s="126">
         <v>0.37994731855487801</v>
       </c>
-      <c r="E43" s="94">
+      <c r="E43" s="79">
         <f>(D43-$D$4)/$D$4</f>
         <v>2.5848951445503624E-3</v>
       </c>
-      <c r="F43" s="52">
+      <c r="F43" s="130">
         <v>0.53449241590238195</v>
       </c>
-      <c r="G43" s="93">
+      <c r="G43" s="78">
         <f>(F43-$F$4)/$F$4</f>
         <v>-6.5656241964681862E-5</v>
       </c>
-      <c r="H43" s="52">
+      <c r="H43" s="130">
         <v>1.2759111725222099E-2</v>
       </c>
-      <c r="I43" s="103">
+      <c r="I43" s="88">
         <f>(H43-$H$4)/$H$4</f>
         <v>-8.5175757490581379E-3</v>
       </c>
@@ -3218,31 +3332,31 @@
       <c r="A44" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="B44" s="60">
+      <c r="B44" s="114">
         <v>0.24431264068346301</v>
       </c>
-      <c r="C44" s="98">
+      <c r="C44" s="83">
         <f>(B44-$B$4)/$B$4</f>
         <v>2.0551540390265658E-3</v>
       </c>
-      <c r="D44" s="54">
+      <c r="D44" s="131">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E44" s="101">
+      <c r="E44" s="86">
         <f>(D44-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F44" s="54">
+      <c r="F44" s="131">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G44" s="101">
+      <c r="G44" s="86">
         <f>(F44-$F$4)/$F$4</f>
         <v>0</v>
       </c>
-      <c r="H44" s="54">
+      <c r="H44" s="131">
         <v>1.2868722039991299E-2</v>
       </c>
-      <c r="I44" s="103">
+      <c r="I44" s="88">
         <f>(H44-$H$4)/$H$4</f>
         <v>0</v>
       </c>
@@ -3251,31 +3365,31 @@
       <c r="A45" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="58">
+      <c r="B45" s="110">
         <v>0.24606974551753799</v>
       </c>
-      <c r="C45" s="97">
+      <c r="C45" s="82">
         <f>(B45-$B$4)/$B$4</f>
         <v>9.2619688409383127E-3</v>
       </c>
-      <c r="D45" s="15">
+      <c r="D45" s="127">
         <v>0.37632945129837098</v>
       </c>
-      <c r="E45" s="99">
+      <c r="E45" s="84">
         <f>(D45-$D$4)/$D$4</f>
         <v>-6.9617416834395346E-3</v>
       </c>
-      <c r="F45" s="65">
+      <c r="F45" s="126">
         <v>0.53565031487291603</v>
       </c>
-      <c r="G45" s="94">
+      <c r="G45" s="79">
         <f>(F45-$F$4)/$F$4</f>
         <v>2.1005540031037331E-3</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="127">
         <v>1.2602666476783E-2</v>
       </c>
-      <c r="I45" s="102">
+      <c r="I45" s="87">
         <f>(H45-$H$4)/$H$4</f>
         <v>-2.0674590870911277E-2</v>
       </c>
@@ -3284,31 +3398,31 @@
       <c r="A46" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="58">
+      <c r="B46" s="110">
         <v>0.244859036420532</v>
       </c>
-      <c r="C46" s="97">
+      <c r="C46" s="82">
         <f>(B46-$B$4)/$B$4</f>
         <v>4.2962114928826517E-3</v>
       </c>
-      <c r="D46" s="65">
+      <c r="D46" s="126">
         <v>0.37994731855487801</v>
       </c>
-      <c r="E46" s="94">
+      <c r="E46" s="79">
         <f>(D46-$D$4)/$D$4</f>
         <v>2.5848951445503624E-3</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="127">
         <v>0.53450270571549696</v>
       </c>
-      <c r="G46" s="99">
+      <c r="G46" s="84">
         <f>(F46-$F$4)/$F$4</f>
         <v>-4.6405945387160456E-5</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H46" s="127">
         <v>1.2756500122734001E-2</v>
       </c>
-      <c r="I46" s="102">
+      <c r="I46" s="87">
         <f>(H46-$H$4)/$H$4</f>
         <v>-8.7205176169439323E-3</v>
       </c>
@@ -3317,31 +3431,31 @@
       <c r="A47" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="60">
+      <c r="B47" s="114">
         <v>0.244307890530198</v>
       </c>
-      <c r="C47" s="98">
+      <c r="C47" s="83">
         <f>(B47-$B$4)/$B$4</f>
         <v>2.035671152065161E-3</v>
       </c>
-      <c r="D47" s="16">
+      <c r="D47" s="132">
         <v>0.37896772671814299</v>
       </c>
-      <c r="E47" s="92">
+      <c r="E47" s="77">
         <f>(D47-$D$4)/$D$4</f>
         <v>0</v>
       </c>
-      <c r="F47" s="16">
+      <c r="F47" s="132">
         <v>0.53452751096997897</v>
       </c>
-      <c r="G47" s="92">
+      <c r="G47" s="77">
         <f>(F47-$F$4)/$F$4</f>
         <v>0</v>
       </c>
-      <c r="H47" s="16">
+      <c r="H47" s="132">
         <v>1.2868722039991299E-2</v>
       </c>
-      <c r="I47" s="102">
+      <c r="I47" s="87">
         <f>(H47-$H$4)/$H$4</f>
         <v>0</v>
       </c>
@@ -3380,7 +3494,7 @@
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection sqref="A1:M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3389,57 +3503,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88" t="s">
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88" t="s">
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88" t="s">
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="137" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106" t="s">
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137" t="s">
         <v>118</v>
       </c>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
-      <c r="K2" s="106" t="s">
+      <c r="I2" s="137"/>
+      <c r="J2" s="137"/>
+      <c r="K2" s="137" t="s">
         <v>119</v>
       </c>
-      <c r="L2" s="106"/>
-      <c r="M2" s="106"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="137"/>
     </row>
     <row r="3" spans="1:13" ht="21" thickBot="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="92" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3480,7 +3594,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="19" thickTop="1">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="93" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="19">
@@ -3494,7 +3608,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="94" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="19">
@@ -3508,27 +3622,27 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="18">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="95" t="s">
         <v>74</v>
       </c>
       <c r="B6" s="19">
         <v>0.22257806244996001</v>
       </c>
-      <c r="C6" s="122">
+      <c r="C6" s="106">
         <v>0.34507606084867798</v>
       </c>
-      <c r="D6" s="122">
+      <c r="D6" s="106">
         <v>0.43634907926340999</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="95" t="s">
         <v>75</v>
       </c>
       <c r="B7" s="19">
         <v>0.22257806244996001</v>
       </c>
-      <c r="C7" s="122">
+      <c r="C7" s="106">
         <v>0.34507606084867798</v>
       </c>
       <c r="D7" s="19">
@@ -3536,7 +3650,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="18">
-      <c r="A8" s="111" t="s">
+      <c r="A8" s="95" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="19">
@@ -3550,7 +3664,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="18">
-      <c r="A9" s="111" t="s">
+      <c r="A9" s="95" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="19">
@@ -3564,7 +3678,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="18">
-      <c r="A10" s="111" t="s">
+      <c r="A10" s="95" t="s">
         <v>78</v>
       </c>
       <c r="B10" s="19">
@@ -3573,18 +3687,18 @@
       <c r="C10" s="19">
         <v>0.34427542033626801</v>
       </c>
-      <c r="D10" s="122">
+      <c r="D10" s="106">
         <v>0.43554843875100002</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="18">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="95" t="s">
         <v>79</v>
       </c>
       <c r="B11" s="19">
         <v>0.22257806244996001</v>
       </c>
-      <c r="C11" s="122">
+      <c r="C11" s="106">
         <v>0.34507606084867798</v>
       </c>
       <c r="D11" s="19">
@@ -3592,21 +3706,21 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="18">
-      <c r="A12" s="111" t="s">
+      <c r="A12" s="95" t="s">
         <v>80</v>
       </c>
       <c r="B12" s="19">
         <v>0.22337870296237</v>
       </c>
-      <c r="C12" s="122">
+      <c r="C12" s="106">
         <v>0.34507606084867798</v>
       </c>
-      <c r="D12" s="122">
+      <c r="D12" s="106">
         <v>0.43554843875100002</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="96" t="s">
         <v>88</v>
       </c>
       <c r="B13" s="19">
@@ -3620,7 +3734,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="18">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="95" t="s">
         <v>89</v>
       </c>
       <c r="B14" s="19">
@@ -3634,7 +3748,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="18">
-      <c r="A15" s="111" t="s">
+      <c r="A15" s="95" t="s">
         <v>90</v>
       </c>
       <c r="B15" s="19">
@@ -3648,7 +3762,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="18">
-      <c r="A16" s="111" t="s">
+      <c r="A16" s="95" t="s">
         <v>91</v>
       </c>
       <c r="B16" s="19">
@@ -3662,7 +3776,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="18">
-      <c r="A17" s="111" t="s">
+      <c r="A17" s="95" t="s">
         <v>92</v>
       </c>
       <c r="B17" s="19">
@@ -3676,7 +3790,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="18">
-      <c r="A18" s="111" t="s">
+      <c r="A18" s="95" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="19">
@@ -3685,12 +3799,12 @@
       <c r="C18" s="19">
         <v>0.34267413931144802</v>
       </c>
-      <c r="D18" s="122">
+      <c r="D18" s="106">
         <v>0.43554843875100002</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="97" t="s">
         <v>94</v>
       </c>
       <c r="B19" s="19">
@@ -3704,7 +3818,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="18">
-      <c r="A20" s="114" t="s">
+      <c r="A20" s="98" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="19">
@@ -3718,7 +3832,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18">
-      <c r="A21" s="115" t="s">
+      <c r="A21" s="99" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="19">
@@ -3732,35 +3846,35 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="18">
-      <c r="A22" s="116" t="s">
+      <c r="A22" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="122">
+      <c r="B22" s="106">
         <v>0.23538831064851801</v>
       </c>
       <c r="C22" s="19">
         <v>0.35068054443554803</v>
       </c>
-      <c r="D22" s="122">
+      <c r="D22" s="106">
         <v>0.44595676541232898</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18">
-      <c r="A23" s="116" t="s">
+      <c r="A23" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="122">
+      <c r="B23" s="106">
         <v>0.23458767013610901</v>
       </c>
       <c r="C23" s="19">
         <v>0.33867093674939902</v>
       </c>
-      <c r="D23" s="122">
+      <c r="D23" s="106">
         <v>0.442754203362689</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18">
-      <c r="A24" s="116" t="s">
+      <c r="A24" s="100" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="19">
@@ -3769,12 +3883,12 @@
       <c r="C24" s="19">
         <v>0.34427542033626801</v>
       </c>
-      <c r="D24" s="122">
+      <c r="D24" s="106">
         <v>0.44035228182545999</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18">
-      <c r="A25" s="116" t="s">
+      <c r="A25" s="100" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="19">
@@ -3783,40 +3897,40 @@
       <c r="C25" s="19">
         <v>0.34427542033626801</v>
       </c>
-      <c r="D25" s="122">
+      <c r="D25" s="106">
         <v>0.44115292233786901</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="100" t="s">
         <v>58</v>
       </c>
       <c r="B26" s="19">
         <v>0.22417934347478</v>
       </c>
-      <c r="C26" s="122">
+      <c r="C26" s="106">
         <v>0.34507606084867798</v>
       </c>
-      <c r="D26" s="122">
+      <c r="D26" s="106">
         <v>0.43634907926340999</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18">
-      <c r="A27" s="116" t="s">
+      <c r="A27" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="122">
+      <c r="B27" s="106">
         <v>0.24339471577261801</v>
       </c>
-      <c r="C27" s="122">
+      <c r="C27" s="106">
         <v>0.353883106485187</v>
       </c>
-      <c r="D27" s="122">
+      <c r="D27" s="106">
         <v>0.44995996797437898</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="100" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="19">
@@ -3825,12 +3939,12 @@
       <c r="C28" s="19">
         <v>0.34427542033626801</v>
       </c>
-      <c r="D28" s="122">
+      <c r="D28" s="106">
         <v>0.44115292233786901</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18">
-      <c r="A29" s="116" t="s">
+      <c r="A29" s="100" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="19">
@@ -3839,68 +3953,68 @@
       <c r="C29" s="19">
         <v>0.33947157726180899</v>
       </c>
-      <c r="D29" s="122">
+      <c r="D29" s="106">
         <v>0.44035228182545999</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="122">
+      <c r="B30" s="106">
         <v>0.23538831064851801</v>
       </c>
       <c r="C30" s="19">
         <v>0.333867093674939</v>
       </c>
-      <c r="D30" s="122">
+      <c r="D30" s="106">
         <v>0.43955164131305002</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18">
-      <c r="A31" s="116" t="s">
+      <c r="A31" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="122">
+      <c r="B31" s="106">
         <v>0.244195356285028</v>
       </c>
-      <c r="C31" s="122">
+      <c r="C31" s="106">
         <v>0.35548438751000699</v>
       </c>
-      <c r="D31" s="122">
+      <c r="D31" s="106">
         <v>0.44595676541232898</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18">
-      <c r="A32" s="116" t="s">
+      <c r="A32" s="100" t="s">
         <v>65</v>
       </c>
       <c r="B32" s="19">
         <v>0.23298638911128899</v>
       </c>
-      <c r="C32" s="122">
+      <c r="C32" s="106">
         <v>0.34747798238590799</v>
       </c>
-      <c r="D32" s="122">
+      <c r="D32" s="106">
         <v>0.44755804643714903</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="122">
+      <c r="B33" s="106">
         <v>0.244195356285028</v>
       </c>
-      <c r="C33" s="122">
+      <c r="C33" s="106">
         <v>0.353883106485188</v>
       </c>
-      <c r="D33" s="122">
+      <c r="D33" s="106">
         <v>0.44835868694955899</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18">
-      <c r="A34" s="117" t="s">
+      <c r="A34" s="101" t="s">
         <v>27</v>
       </c>
       <c r="B34" s="19">
@@ -3909,12 +4023,12 @@
       <c r="C34" s="19">
         <v>0.34427542033626801</v>
       </c>
-      <c r="D34" s="122">
+      <c r="D34" s="106">
         <v>0.44115292233786901</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18">
-      <c r="A35" s="118" t="s">
+      <c r="A35" s="102" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="19">
@@ -3923,18 +4037,18 @@
       <c r="C35" s="19">
         <v>0.333867093674939</v>
       </c>
-      <c r="D35" s="122">
+      <c r="D35" s="106">
         <v>0.44035228182545999</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18">
-      <c r="A36" s="119" t="s">
+      <c r="A36" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="122">
+      <c r="B36" s="106">
         <v>0.22978382706164899</v>
       </c>
-      <c r="C36" s="122">
+      <c r="C36" s="106">
         <v>0.34747798238590799</v>
       </c>
       <c r="D36" s="19">
@@ -3942,13 +4056,13 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="18">
-      <c r="A37" s="118" t="s">
+      <c r="A37" s="102" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="19">
         <v>0.21457165732586</v>
       </c>
-      <c r="C37" s="122">
+      <c r="C37" s="106">
         <v>0.34907926341072798</v>
       </c>
       <c r="D37" s="19">
@@ -3956,7 +4070,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="18">
-      <c r="A38" s="118" t="s">
+      <c r="A38" s="102" t="s">
         <v>71</v>
       </c>
       <c r="B38" s="19">
@@ -3970,7 +4084,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="18">
-      <c r="A39" s="118" t="s">
+      <c r="A39" s="102" t="s">
         <v>51</v>
       </c>
       <c r="B39" s="19">
@@ -3984,7 +4098,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18">
-      <c r="A40" s="119" t="s">
+      <c r="A40" s="103" t="s">
         <v>52</v>
       </c>
       <c r="B40" s="19">
@@ -3998,21 +4112,21 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="18">
-      <c r="A41" s="118" t="s">
+      <c r="A41" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="122">
+      <c r="B41" s="106">
         <v>0.23058446757405901</v>
       </c>
       <c r="C41" s="19">
         <v>0.34667734187349802</v>
       </c>
-      <c r="D41" s="122">
+      <c r="D41" s="106">
         <v>0.44275420336269</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="104" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="19">
@@ -4021,40 +4135,40 @@
       <c r="C42" s="19">
         <v>0.34027221777421901</v>
       </c>
-      <c r="D42" s="122">
+      <c r="D42" s="106">
         <v>0.43875100080064</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="122">
+      <c r="B43" s="106">
         <v>0.23298638911128899</v>
       </c>
       <c r="C43" s="19">
         <v>0.34267413931144802</v>
       </c>
-      <c r="D43" s="122">
+      <c r="D43" s="106">
         <v>0.44435548438750899</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18">
-      <c r="A44" s="121" t="s">
+      <c r="A44" s="105" t="s">
         <v>69</v>
       </c>
       <c r="B44" s="19">
         <v>0.22337870296237</v>
       </c>
-      <c r="C44" s="122">
+      <c r="C44" s="106">
         <v>0.34907926341072798</v>
       </c>
-      <c r="D44" s="122">
+      <c r="D44" s="106">
         <v>0.43875100080064</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18">
-      <c r="A45" s="117" t="s">
+      <c r="A45" s="101" t="s">
         <v>68</v>
       </c>
       <c r="B45" s="19">
@@ -4068,7 +4182,7 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="18">
-      <c r="A46" s="119" t="s">
+      <c r="A46" s="103" t="s">
         <v>32</v>
       </c>
       <c r="B46" s="19">
@@ -4077,12 +4191,12 @@
       <c r="C46" s="19">
         <v>0.34507606084867798</v>
       </c>
-      <c r="D46" s="122">
+      <c r="D46" s="106">
         <v>0.44115292233787001</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18">
-      <c r="A47" s="118" t="s">
+      <c r="A47" s="102" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="19">
@@ -4091,12 +4205,12 @@
       <c r="C47" s="19">
         <v>0.34907926341072798</v>
       </c>
-      <c r="D47" s="122">
+      <c r="D47" s="106">
         <v>0.43875100080064</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18">
-      <c r="A48" s="120" t="s">
+      <c r="A48" s="104" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="19">
@@ -4111,14 +4225,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K2:M2"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:B48">
     <cfRule type="colorScale" priority="3">
@@ -4171,7 +4285,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4233,7 +4347,7 @@
       <c r="C4" s="2">
         <v>222</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="75">
         <v>5.6261261261261204</v>
       </c>
       <c r="E4" s="19">
@@ -4263,7 +4377,7 @@
       <c r="C5" s="2">
         <v>35</v>
       </c>
-      <c r="D5" s="90">
+      <c r="D5" s="75">
         <v>4.8571428571428497</v>
       </c>
       <c r="E5" s="19">
@@ -4293,7 +4407,7 @@
       <c r="C6" s="2">
         <v>30</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="75">
         <v>23.2</v>
       </c>
       <c r="E6" s="19">
@@ -4323,7 +4437,7 @@
       <c r="C7" s="2">
         <v>83</v>
       </c>
-      <c r="D7" s="90">
+      <c r="D7" s="75">
         <v>3.9036144578313201</v>
       </c>
       <c r="E7" s="19">
@@ -4559,10 +4673,10 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="86">
+      <c r="B21" s="72">
         <v>2.1849105974699998E-2</v>
       </c>
-      <c r="C21" s="86">
+      <c r="C21" s="72">
         <v>4.4785264713399997E-2</v>
       </c>
     </row>
@@ -4576,13 +4690,13 @@
       <c r="C23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="87"/>
+      <c r="E23" s="73"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="86">
+      <c r="B24" s="72">
         <v>0.5746</v>
       </c>
-      <c r="C24" s="86">
+      <c r="C24" s="72">
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
@@ -4743,7 +4857,7 @@
         <f t="shared" si="1"/>
         <v>-1.4136145321746885E-3</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="62">
         <v>0.53529098731159497</v>
       </c>
       <c r="G5" s="55">
@@ -4927,7 +5041,7 @@
       <c r="A11" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="69">
+      <c r="B11" s="58">
         <v>0.28221558750820902</v>
       </c>
       <c r="C11" s="55">
@@ -4981,7 +5095,7 @@
         <f t="shared" si="2"/>
         <v>-6.7323011412058195E-2</v>
       </c>
-      <c r="H12" s="77">
+      <c r="H12" s="66">
         <v>1.380620281143E-2</v>
       </c>
       <c r="I12" s="57">
@@ -5000,7 +5114,7 @@
         <f t="shared" si="0"/>
         <v>-2.1409224341782931E-3</v>
       </c>
-      <c r="D13" s="72">
+      <c r="D13" s="61">
         <v>0.38526070879256302</v>
       </c>
       <c r="E13" s="56">
@@ -5026,21 +5140,21 @@
       <c r="A14" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="69">
+      <c r="B14" s="58">
         <v>0.29653734494720901</v>
       </c>
       <c r="C14" s="55">
         <f t="shared" si="0"/>
         <v>5.182636306283174E-2</v>
       </c>
-      <c r="D14" s="73">
+      <c r="D14" s="62">
         <v>0.38438913315652201</v>
       </c>
       <c r="E14" s="55">
         <f t="shared" si="1"/>
         <v>1.4305720662095284E-2</v>
       </c>
-      <c r="F14" s="73">
+      <c r="F14" s="62">
         <v>0.55367549907609603</v>
       </c>
       <c r="G14" s="55">
@@ -5059,7 +5173,7 @@
       <c r="A15" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="70">
+      <c r="B15" s="59">
         <v>0.288927228692064</v>
       </c>
       <c r="C15" s="55">
@@ -5073,7 +5187,7 @@
         <f t="shared" si="1"/>
         <v>-7.5601350334265503E-4</v>
       </c>
-      <c r="F15" s="74">
+      <c r="F15" s="63">
         <v>0.54996186535253899</v>
       </c>
       <c r="G15" s="55">
@@ -5092,7 +5206,7 @@
       <c r="A16" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="70">
+      <c r="B16" s="59">
         <v>0.29046785478988502</v>
       </c>
       <c r="C16" s="55">
@@ -5113,7 +5227,7 @@
         <f t="shared" si="2"/>
         <v>2.1145887959988691E-4</v>
       </c>
-      <c r="H16" s="74">
+      <c r="H16" s="63">
         <v>1.35859384549026E-2</v>
       </c>
       <c r="I16" s="57">
@@ -5125,7 +5239,7 @@
       <c r="A17" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="70">
+      <c r="B17" s="59">
         <v>0.28415653055485501</v>
       </c>
       <c r="C17" s="55">
@@ -5139,14 +5253,14 @@
         <f t="shared" si="1"/>
         <v>-6.008862852346906E-3</v>
       </c>
-      <c r="F17" s="74">
+      <c r="F17" s="63">
         <v>0.53532905335487102</v>
       </c>
       <c r="G17" s="55">
         <f t="shared" si="2"/>
         <v>1.4995343896098711E-3</v>
       </c>
-      <c r="H17" s="74">
+      <c r="H17" s="63">
         <v>1.30183920223378E-2</v>
       </c>
       <c r="I17" s="57">
@@ -5158,21 +5272,21 @@
       <c r="A18" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="70">
+      <c r="B18" s="59">
         <v>0.28248171119676901</v>
       </c>
       <c r="C18" s="55">
         <f t="shared" si="0"/>
         <v>1.9706319713551235E-3</v>
       </c>
-      <c r="D18" s="74">
+      <c r="D18" s="63">
         <v>0.37988381547669597</v>
       </c>
       <c r="E18" s="55">
         <f t="shared" si="1"/>
         <v>2.4173265794591534E-3</v>
       </c>
-      <c r="F18" s="74">
+      <c r="F18" s="63">
         <v>0.53574071266044399</v>
       </c>
       <c r="G18" s="55">
@@ -5191,21 +5305,21 @@
       <c r="A19" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="70">
+      <c r="B19" s="59">
         <v>0.29743571600449498</v>
       </c>
       <c r="C19" s="55">
         <f t="shared" si="0"/>
         <v>5.501291065276253E-2</v>
       </c>
-      <c r="D19" s="74">
+      <c r="D19" s="63">
         <v>0.39641490169830002</v>
       </c>
       <c r="E19" s="55">
         <f t="shared" si="1"/>
         <v>4.6038682848403463E-2</v>
       </c>
-      <c r="F19" s="74">
+      <c r="F19" s="63">
         <v>0.54917346358164898</v>
       </c>
       <c r="G19" s="55">
@@ -5224,7 +5338,7 @@
       <c r="A20" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="70">
+      <c r="B20" s="59">
         <v>0.28449176618636801</v>
       </c>
       <c r="C20" s="55">
@@ -5257,7 +5371,7 @@
       <c r="A21" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="69">
+      <c r="B21" s="58">
         <v>0.29268604756354599</v>
       </c>
       <c r="C21" s="55">
@@ -5271,14 +5385,14 @@
         <f t="shared" si="1"/>
         <v>-2.2236940182881627E-2</v>
       </c>
-      <c r="F21" s="73">
+      <c r="F21" s="62">
         <v>0.53937298891714602</v>
       </c>
       <c r="G21" s="55">
         <f t="shared" si="2"/>
         <v>9.0649739213127124E-3</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="62">
         <v>1.3648952584519701E-2</v>
       </c>
       <c r="I21" s="57">
@@ -5290,7 +5404,7 @@
       <c r="A22" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="69">
+      <c r="B22" s="58">
         <v>0.29014039682978898</v>
       </c>
       <c r="C22" s="55">
@@ -5304,7 +5418,7 @@
         <f t="shared" si="1"/>
         <v>-7.2788512188832132E-4</v>
       </c>
-      <c r="F22" s="73">
+      <c r="F22" s="62">
         <v>0.54993468130357903</v>
       </c>
       <c r="G22" s="55">
@@ -5323,21 +5437,21 @@
       <c r="A23" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="69">
+      <c r="B23" s="58">
         <v>0.29759868495102298</v>
       </c>
       <c r="C23" s="55">
         <f t="shared" si="0"/>
         <v>5.5590966122805445E-2</v>
       </c>
-      <c r="D23" s="73">
+      <c r="D23" s="62">
         <v>0.39726774857955199</v>
       </c>
       <c r="E23" s="55">
         <f t="shared" si="1"/>
         <v>4.8289130105845741E-2</v>
       </c>
-      <c r="F23" s="73">
+      <c r="F23" s="62">
         <v>0.546802537990702</v>
       </c>
       <c r="G23" s="55">
@@ -5356,21 +5470,21 @@
       <c r="A24" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="69">
+      <c r="B24" s="58">
         <v>0.29107029321505701</v>
       </c>
       <c r="C24" s="55">
         <f t="shared" si="0"/>
         <v>3.2434575694095732E-2</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D24" s="62">
         <v>0.39310991873477502</v>
       </c>
       <c r="E24" s="55">
         <f t="shared" si="1"/>
         <v>3.7317668549518131E-2</v>
       </c>
-      <c r="F24" s="73">
+      <c r="F24" s="62">
         <v>0.54872729136451703</v>
       </c>
       <c r="G24" s="55">
@@ -5390,21 +5504,21 @@
       <c r="A25" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="69">
+      <c r="B25" s="58">
         <v>0.29731305946279801</v>
       </c>
       <c r="C25" s="55">
         <f t="shared" si="0"/>
         <v>5.4577844424655748E-2</v>
       </c>
-      <c r="D25" s="73">
+      <c r="D25" s="62">
         <v>0.40030732402595998</v>
       </c>
       <c r="E25" s="55">
         <f t="shared" si="1"/>
         <v>5.6309801081526646E-2</v>
       </c>
-      <c r="F25" s="73">
+      <c r="F25" s="62">
         <v>0.54750841525724203</v>
       </c>
       <c r="G25" s="55">
@@ -5423,7 +5537,7 @@
       <c r="A26" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="71">
+      <c r="B26" s="60">
         <v>0.28465564794916498</v>
       </c>
       <c r="C26" s="56">
@@ -5437,14 +5551,14 @@
         <f t="shared" si="1"/>
         <v>-8.1734777744747709E-3</v>
       </c>
-      <c r="F26" s="76">
+      <c r="F26" s="65">
         <v>0.53622283927042402</v>
       </c>
       <c r="G26" s="56">
         <f t="shared" si="2"/>
         <v>3.1716390001491797E-3</v>
       </c>
-      <c r="H26" s="76">
+      <c r="H26" s="65">
         <v>1.31215634397718E-2</v>
       </c>
       <c r="I26" s="57">
@@ -5489,7 +5603,7 @@
       <c r="A28" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="69">
+      <c r="B28" s="58">
         <v>0.28416999852125602</v>
       </c>
       <c r="C28" s="55">
@@ -5529,14 +5643,14 @@
         <f t="shared" si="0"/>
         <v>-8.1968158837011605E-3</v>
       </c>
-      <c r="D29" s="75">
+      <c r="D29" s="64">
         <v>0.38296243580524197</v>
       </c>
       <c r="E29" s="55">
         <f t="shared" si="1"/>
         <v>1.0541027125695171E-2</v>
       </c>
-      <c r="F29" s="75">
+      <c r="F29" s="64">
         <v>0.53701945475882096</v>
       </c>
       <c r="G29" s="55">
@@ -5576,10 +5690,10 @@
         <f t="shared" si="2"/>
         <v>-4.1517792743384921E-2</v>
       </c>
-      <c r="H30" s="79">
+      <c r="H30" s="68">
         <v>1.31626912160602E-2</v>
       </c>
-      <c r="I30" s="80">
+      <c r="I30" s="69">
         <f t="shared" si="3"/>
         <v>2.2843696146000476E-2</v>
       </c>
@@ -5628,24 +5742,24 @@
         <f t="shared" si="0"/>
         <v>-9.2025636544072788E-3</v>
       </c>
-      <c r="D32" s="75">
+      <c r="D32" s="64">
         <v>0.383255982113542</v>
       </c>
       <c r="E32" s="55">
         <f t="shared" si="1"/>
         <v>1.1315621603283378E-2</v>
       </c>
-      <c r="F32" s="75">
+      <c r="F32" s="64">
         <v>0.53673611445874703</v>
       </c>
       <c r="G32" s="55">
         <f t="shared" si="2"/>
         <v>4.1318799190713691E-3</v>
       </c>
-      <c r="H32" s="75">
+      <c r="H32" s="64">
         <v>1.29005175033796E-2</v>
       </c>
-      <c r="I32" s="80">
+      <c r="I32" s="69">
         <f t="shared" si="3"/>
         <v>2.4707553158341881E-3</v>
       </c>
@@ -5661,7 +5775,7 @@
         <f t="shared" si="0"/>
         <v>-2.0892274417673388E-3</v>
       </c>
-      <c r="D33" s="75">
+      <c r="D33" s="64">
         <v>0.39407782295149602</v>
       </c>
       <c r="E33" s="55">
@@ -5701,7 +5815,7 @@
         <f t="shared" si="1"/>
         <v>5.078500128472517E-3</v>
       </c>
-      <c r="F34" s="78">
+      <c r="F34" s="67">
         <v>0.53545832037546803</v>
       </c>
       <c r="G34" s="56">
@@ -5734,7 +5848,7 @@
         <f t="shared" si="1"/>
         <v>-7.2654921934363105E-3</v>
       </c>
-      <c r="F35" s="75">
+      <c r="F35" s="64">
         <v>0.53516201806589503</v>
       </c>
       <c r="G35" s="55">
@@ -5753,14 +5867,14 @@
       <c r="A36" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="69">
+      <c r="B36" s="58">
         <v>0.28288709137675999</v>
       </c>
       <c r="C36" s="55">
         <f t="shared" si="0"/>
         <v>3.4085269537006816E-3</v>
       </c>
-      <c r="D36" s="75">
+      <c r="D36" s="64">
         <v>0.38397906458662401</v>
       </c>
       <c r="E36" s="55">
@@ -5819,7 +5933,7 @@
       <c r="A38" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="69">
+      <c r="B38" s="58">
         <v>0.28431155603143099</v>
       </c>
       <c r="C38" s="55">
@@ -5833,7 +5947,7 @@
         <f t="shared" si="1"/>
         <v>-6.9617416834395346E-3</v>
       </c>
-      <c r="F38" s="75">
+      <c r="F38" s="64">
         <v>0.53565031487291603</v>
       </c>
       <c r="G38" s="55">
@@ -5852,14 +5966,14 @@
       <c r="A39" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="69">
+      <c r="B39" s="58">
         <v>0.28245202296716598</v>
       </c>
       <c r="C39" s="55">
         <f t="shared" si="0"/>
         <v>1.8653269799224607E-3</v>
       </c>
-      <c r="D39" s="75">
+      <c r="D39" s="64">
         <v>0.38397906458662401</v>
       </c>
       <c r="E39" s="55">

</xml_diff>